<commit_message>
Rw Usage Updates S.1.0.0.3 _8:00PM
Boat Enabled -
InCapacity - [13] , NodeW - [-3] , BirdW - [6] , FuelW - [19] , OnHost - [5]
VillageW=[5]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.8.xlsx
+++ b/Usage_S_1.0.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4D7A90-AC13-44C3-8FF6-57E95A19851F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6E984E-53B3-4175-B5F7-42C566809E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="226">
   <si>
     <t>UnSettled</t>
   </si>
@@ -711,13 +711,16 @@
   </si>
   <si>
     <t>RA</t>
+  </si>
+  <si>
+    <t>X-Professional - (7)-X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,6 +883,14 @@
     <font>
       <sz val="8"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFD515BA"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1599,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="289">
+  <cellXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2174,6 +2185,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2210,6 +2233,45 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2234,61 +2296,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2302,27 +2322,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2331,6 +2346,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD515BA"/>
       <color rgb="FFF385E3"/>
     </mruColors>
   </colors>
@@ -2611,7 +2627,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,15 +2664,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="243">
+      <c r="C2" s="247">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="247" t="s">
+      <c r="E2" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="248"/>
-      <c r="G2" s="249"/>
+      <c r="F2" s="252"/>
+      <c r="G2" s="253"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2705,19 +2721,19 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="245" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="244"/>
+      <c r="C3" s="248"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="242"/>
+      <c r="A4" s="246"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -2727,7 +2743,9 @@
       <c r="E4" s="140">
         <v>10</v>
       </c>
-      <c r="F4" s="205"/>
+      <c r="F4" s="205">
+        <v>10</v>
+      </c>
       <c r="G4" s="164"/>
       <c r="H4" s="9" t="s">
         <v>199</v>
@@ -2757,12 +2775,12 @@
         <v>30</v>
       </c>
       <c r="Q4" s="154">
-        <v>0.66666666666666663</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="S4" s="154">
-        <v>0.85555555555555562</v>
-      </c>
-      <c r="T4" s="287">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="T4" s="240">
         <v>3</v>
       </c>
       <c r="U4" s="24" t="s">
@@ -2770,7 +2788,9 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
       <c r="D5" s="156">
         <v>-2</v>
       </c>
@@ -2812,7 +2832,7 @@
       <c r="S5" s="154">
         <v>0.85555555555555562</v>
       </c>
-      <c r="T5" s="285">
+      <c r="T5" s="238">
         <v>1</v>
       </c>
       <c r="U5" s="24" t="s">
@@ -2821,10 +2841,10 @@
     </row>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>2245</v>
+        <v>2325</v>
       </c>
       <c r="C6">
-        <v>6730</v>
+        <v>6650</v>
       </c>
       <c r="E6" s="218">
         <v>10</v>
@@ -2864,7 +2884,7 @@
       <c r="S6" s="154">
         <v>0.85555555555555562</v>
       </c>
-      <c r="T6" s="287">
+      <c r="T6" s="240">
         <v>3</v>
       </c>
       <c r="U6" s="24" t="s">
@@ -2881,7 +2901,9 @@
       <c r="E7" s="165">
         <v>10</v>
       </c>
-      <c r="F7" s="207"/>
+      <c r="F7" s="289">
+        <v>10</v>
+      </c>
       <c r="G7" s="127"/>
       <c r="H7" s="9" t="s">
         <v>188</v>
@@ -2911,15 +2933,15 @@
         <v>95</v>
       </c>
       <c r="Q7" s="154">
-        <v>0.66666666666666663</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>130</v>
       </c>
       <c r="S7" s="154">
-        <v>0.85555555555555562</v>
-      </c>
-      <c r="T7" s="287">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="T7" s="240">
         <v>3</v>
       </c>
       <c r="U7" s="24" t="s">
@@ -2928,7 +2950,9 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="219"/>
-      <c r="F8" s="208"/>
+      <c r="F8" s="289">
+        <v>35</v>
+      </c>
       <c r="G8" s="190"/>
       <c r="H8" s="9" t="s">
         <v>72</v>
@@ -2937,7 +2961,9 @@
         <v>17</v>
       </c>
       <c r="J8" s="213"/>
-      <c r="K8" s="194"/>
+      <c r="K8" s="194" t="s">
+        <v>225</v>
+      </c>
       <c r="L8" s="83" t="s">
         <v>214</v>
       </c>
@@ -2954,14 +2980,16 @@
         <v>65</v>
       </c>
       <c r="Q8" s="154">
-        <v>0.8125</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="S8" s="154">
-        <v>0.85555555555555562</v>
-      </c>
-      <c r="T8" s="24"/>
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="T8" s="240">
+        <v>3</v>
+      </c>
       <c r="U8" s="24" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2970,7 +2998,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>9245</v>
+        <v>9325</v>
       </c>
       <c r="E9" s="163">
         <v>14</v>
@@ -2986,7 +3014,7 @@
       <c r="J9" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K9" s="215" t="s">
+      <c r="K9" s="169" t="s">
         <v>215</v>
       </c>
       <c r="L9" s="223" t="s">
@@ -3010,7 +3038,7 @@
       <c r="S9" s="154">
         <v>0.71875</v>
       </c>
-      <c r="T9" s="286">
+      <c r="T9" s="239">
         <v>1</v>
       </c>
       <c r="U9" s="24" t="s">
@@ -3019,7 +3047,9 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="220"/>
-      <c r="F10" s="165"/>
+      <c r="F10" s="206">
+        <v>10</v>
+      </c>
       <c r="G10" s="177"/>
       <c r="H10" s="9" t="s">
         <v>81</v>
@@ -3028,7 +3058,6 @@
         <v>17</v>
       </c>
       <c r="J10" s="213"/>
-      <c r="K10" s="169"/>
       <c r="L10" s="83" t="s">
         <v>143</v>
       </c>
@@ -3045,14 +3074,16 @@
         <v>66</v>
       </c>
       <c r="Q10" s="154">
-        <v>0.8125</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="S10" s="154">
-        <v>0.84375</v>
-      </c>
-      <c r="T10" s="24"/>
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="T10" s="240">
+        <v>6</v>
+      </c>
       <c r="U10" s="24" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3066,7 +3097,9 @@
       <c r="E11" s="221">
         <v>5</v>
       </c>
-      <c r="F11" s="209"/>
+      <c r="F11" s="289">
+        <v>15</v>
+      </c>
       <c r="G11" s="184"/>
       <c r="H11" s="9" t="s">
         <v>102</v>
@@ -3096,12 +3129,15 @@
         <v>161</v>
       </c>
       <c r="Q11" s="154">
-        <v>0.66666666666666663</v>
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="S11" s="154">
-        <v>0.8125</v>
-      </c>
-      <c r="T11" s="288">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="T11" s="241">
         <v>1</v>
       </c>
       <c r="U11" s="24" t="s">
@@ -3146,7 +3182,7 @@
       <c r="S12" s="154">
         <v>0.84375</v>
       </c>
-      <c r="T12" s="285">
+      <c r="T12" s="238">
         <v>3</v>
       </c>
       <c r="U12" s="24" t="s">
@@ -3159,7 +3195,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>9245</v>
+        <v>9325</v>
       </c>
       <c r="E13" s="36">
         <v>1</v>
@@ -3200,7 +3236,6 @@
       <c r="S13" s="154">
         <v>0.84375</v>
       </c>
-      <c r="T13" s="24"/>
       <c r="U13" s="24" t="s">
         <v>223</v>
       </c>
@@ -3241,7 +3276,6 @@
       <c r="S14" s="154">
         <v>0.91666666666666663</v>
       </c>
-      <c r="T14" s="24"/>
       <c r="U14" s="24" t="s">
         <v>223</v>
       </c>
@@ -3276,9 +3310,7 @@
       <c r="Q15" s="154">
         <v>0.91666666666666663</v>
       </c>
-      <c r="R15" t="s">
-        <v>126</v>
-      </c>
+      <c r="R15"/>
       <c r="S15" s="154">
         <v>0.91666666666666663</v>
       </c>
@@ -3298,21 +3330,21 @@
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="245" t="s">
+      <c r="E17" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="246"/>
+      <c r="F17" s="250"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>330</v>
+        <v>410</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="216"/>
       <c r="L17" s="119"/>
-      <c r="Q17" s="239"/>
-      <c r="R17" s="240"/>
+      <c r="Q17" s="243"/>
+      <c r="R17" s="244"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -3330,14 +3362,14 @@
       <c r="J18" s="119"/>
       <c r="K18" s="216"/>
       <c r="L18" s="119"/>
-      <c r="M18" s="238"/>
-      <c r="Q18" s="239"/>
-      <c r="R18" s="240"/>
+      <c r="M18" s="242"/>
+      <c r="Q18" s="243"/>
+      <c r="R18" s="244"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="238"/>
+      <c r="M19" s="242"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="227"/>
@@ -3360,10 +3392,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R41" sqref="R41"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3387,18 +3419,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="250" t="s">
+      <c r="E1" s="267" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="252"/>
+      <c r="F1" s="269"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="250" t="s">
+      <c r="H1" s="267" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="251"/>
-      <c r="J1" s="252"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="269"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3416,7 +3448,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="253">
+      <c r="B2" s="270">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -3443,26 +3475,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="256">
+      <c r="K2" s="273">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="271">
+      <c r="L2" s="264">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="261">
+      <c r="M2" s="254">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J53)</f>
-        <v>9205</v>
+        <f>SUM(E2:J54)</f>
+        <v>9285</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="254"/>
+      <c r="B3" s="271"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3477,13 +3509,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="257"/>
-      <c r="L3" s="272"/>
-      <c r="M3" s="262"/>
+      <c r="K3" s="274"/>
+      <c r="L3" s="265"/>
+      <c r="M3" s="255"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="255"/>
+      <c r="B4" s="272"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3498,9 +3530,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="272"/>
-      <c r="M4" s="262"/>
+      <c r="K4" s="274"/>
+      <c r="L4" s="265"/>
+      <c r="M4" s="255"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -3582,7 +3614,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="263">
+      <c r="B7" s="256">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -3599,22 +3631,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="265">
+      <c r="K7" s="258">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="267">
+      <c r="L7" s="260">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="269">
+      <c r="M7" s="262">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="264"/>
+      <c r="B8" s="257"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -3635,9 +3667,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="266"/>
-      <c r="L8" s="268"/>
-      <c r="M8" s="270"/>
+      <c r="K8" s="259"/>
+      <c r="L8" s="261"/>
+      <c r="M8" s="263"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -3717,7 +3749,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="263">
+      <c r="B11" s="256">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3744,7 +3776,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="264"/>
+      <c r="B12" s="257"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3801,7 +3833,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="263">
+      <c r="B14" s="256">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3824,7 +3856,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="264"/>
+      <c r="B15" s="257"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3848,7 +3880,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="253">
+      <c r="B16" s="270">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3879,7 +3911,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="254"/>
+      <c r="B17" s="271"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3897,7 +3929,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="253">
+      <c r="B18" s="270">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3926,7 +3958,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="255"/>
+      <c r="B19" s="272"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3986,7 +4018,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="259">
+      <c r="B21" s="275">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4014,7 +4046,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="260"/>
+      <c r="B22" s="276"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4066,7 +4098,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="243">
+      <c r="B24" s="247">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -4095,7 +4127,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="244"/>
+      <c r="B25" s="248"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -4123,7 +4155,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="243">
+      <c r="B26" s="247">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -4154,7 +4186,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="258"/>
+      <c r="B27" s="266"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4185,7 +4217,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="243">
+      <c r="B28" s="247">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -4207,7 +4239,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="244"/>
+      <c r="B29" s="248"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -4233,7 +4265,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="243">
+      <c r="B30" s="247">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -4256,7 +4288,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="244"/>
+      <c r="B31" s="248"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4283,7 +4315,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="243">
+      <c r="B32" s="247">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -4305,7 +4337,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="244"/>
+      <c r="B33" s="248"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4358,7 +4390,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="243">
+      <c r="B35" s="247">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -4385,7 +4417,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="244"/>
+      <c r="B36" s="248"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -4407,7 +4439,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="243">
+      <c r="B37" s="247">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -4440,7 +4472,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="244"/>
+      <c r="B38" s="248"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -4458,7 +4490,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="243">
+      <c r="B39" s="247">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -4485,7 +4517,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="258"/>
+      <c r="B40" s="266"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -4513,7 +4545,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="243">
+      <c r="B41" s="247">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -4540,7 +4572,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="258"/>
+      <c r="B42" s="266"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -4558,7 +4590,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="244"/>
+      <c r="B43" s="248"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -4587,7 +4619,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="243">
+      <c r="B44" s="247">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -4613,7 +4645,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="244"/>
+      <c r="B45" s="248"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -4638,7 +4670,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="243">
+      <c r="B46" s="247">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -4660,7 +4692,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="258"/>
+      <c r="B47" s="266"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -4681,7 +4713,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="243">
+      <c r="B48" s="247">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -4701,7 +4733,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="258"/>
+      <c r="B49" s="266"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -4727,7 +4759,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="258"/>
+      <c r="B50" s="266"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -4754,7 +4786,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="243">
+      <c r="B51" s="247">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -4776,7 +4808,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="244"/>
+      <c r="B52" s="248"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -4803,10 +4835,10 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="130">
+      <c r="B53" s="247">
         <v>30</v>
       </c>
-      <c r="C53" s="18"/>
+      <c r="C53" s="142"/>
       <c r="D53" s="18">
         <v>330</v>
       </c>
@@ -4830,20 +4862,27 @@
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
     </row>
+    <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="248"/>
+      <c r="C54" s="142"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="290">
+        <v>60</v>
+      </c>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="290">
+        <v>20</v>
+      </c>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B44:B45"/>
+  <mergeCells count="29">
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="K2:K4"/>
@@ -4860,6 +4899,18 @@
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B35:B36"/>
     <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B44:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8066,10 +8117,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="245" t="s">
+      <c r="AG24" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="246"/>
+      <c r="AH24" s="250"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -8089,10 +8140,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="245" t="s">
+      <c r="AZ24" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="246"/>
+      <c r="BA24" s="250"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -8112,10 +8163,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="245" t="s">
+      <c r="BR24" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="246"/>
+      <c r="BS24" s="250"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -8138,10 +8189,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="247" t="s">
+      <c r="B26" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="249"/>
+      <c r="C26" s="253"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8178,10 +8229,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="247" t="s">
+      <c r="R26" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="249"/>
+      <c r="S26" s="253"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8218,10 +8269,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="247" t="s">
+      <c r="AG26" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="249"/>
+      <c r="AH26" s="253"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8258,10 +8309,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="247" t="s">
+      <c r="AW26" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="249"/>
+      <c r="AX26" s="253"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8298,10 +8349,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="247" t="s">
+      <c r="BM26" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="249"/>
+      <c r="BN26" s="253"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9295,7 +9346,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="282">
+      <c r="AX32" s="277">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -9333,7 +9384,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="282">
+      <c r="BN32" s="277">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -9482,7 +9533,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="283"/>
+      <c r="AX33" s="278"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9518,7 +9569,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="283"/>
+      <c r="BN33" s="278"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9669,7 +9720,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="284"/>
+      <c r="AX34" s="279"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9707,7 +9758,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="284"/>
+      <c r="BN34" s="279"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9938,10 +9989,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="245" t="s">
+      <c r="B36" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="246"/>
+      <c r="C36" s="250"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -9959,10 +10010,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="245" t="s">
+      <c r="R36" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="246"/>
+      <c r="S36" s="250"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -9980,10 +10031,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="245" t="s">
+      <c r="AG36" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="246"/>
+      <c r="AH36" s="250"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -10001,10 +10052,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="245" t="s">
+      <c r="AW36" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="246"/>
+      <c r="AX36" s="250"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -10022,10 +10073,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="245" t="s">
+      <c r="BM36" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="246"/>
+      <c r="BN36" s="250"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -10045,10 +10096,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="247" t="s">
+      <c r="B38" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="249"/>
+      <c r="C38" s="253"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10088,10 +10139,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="247" t="s">
+      <c r="S38" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="249"/>
+      <c r="T38" s="253"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10131,11 +10182,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="247" t="s">
+      <c r="AJ38" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="248"/>
-      <c r="AL38" s="249"/>
+      <c r="AK38" s="252"/>
+      <c r="AL38" s="253"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10180,11 +10231,11 @@
         <f ca="1">TODAY()</f>
         <v>45290</v>
       </c>
-      <c r="BD38" s="247" t="s">
+      <c r="BD38" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="248"/>
-      <c r="BF38" s="249"/>
+      <c r="BE38" s="252"/>
+      <c r="BF38" s="253"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10224,11 +10275,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="247" t="s">
+      <c r="BW38" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="248"/>
-      <c r="BY38" s="249"/>
+      <c r="BX38" s="252"/>
+      <c r="BY38" s="253"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11180,7 +11231,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="282">
+      <c r="C44" s="277">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -11218,10 +11269,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="275">
+      <c r="S44" s="286">
         <v>25</v>
       </c>
-      <c r="T44" s="282">
+      <c r="T44" s="277">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -11230,7 +11281,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="277" t="s">
+      <c r="W44" s="280" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -11259,10 +11310,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="275">
+      <c r="AJ44" s="286">
         <v>50</v>
       </c>
-      <c r="AK44" s="282">
+      <c r="AK44" s="277">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -11272,7 +11323,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="277" t="s">
+      <c r="AO44" s="280" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -11302,7 +11353,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="275">
+      <c r="BD44" s="286">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -11313,7 +11364,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="277" t="s">
+      <c r="BI44" s="280" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -11342,7 +11393,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="275">
+      <c r="BW44" s="286">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -11353,7 +11404,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="277" t="s">
+      <c r="CB44" s="280" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -11385,7 +11436,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="283"/>
+      <c r="C45" s="278"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -11419,15 +11470,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="276"/>
-      <c r="T45" s="284"/>
+      <c r="S45" s="287"/>
+      <c r="T45" s="279"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="278"/>
+      <c r="W45" s="281"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11454,8 +11505,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="276"/>
-      <c r="AK45" s="284"/>
+      <c r="AJ45" s="287"/>
+      <c r="AK45" s="279"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -11463,7 +11514,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="278"/>
+      <c r="AO45" s="281"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11491,7 +11542,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="276"/>
+      <c r="BD45" s="287"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -11502,7 +11553,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="278"/>
+      <c r="BI45" s="281"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11529,7 +11580,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="276"/>
+      <c r="BW45" s="287"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -11538,7 +11589,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="278"/>
+      <c r="CB45" s="281"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11568,7 +11619,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="284"/>
+      <c r="C46" s="279"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -11995,10 +12046,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="245" t="s">
+      <c r="B48" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="246"/>
+      <c r="C48" s="250"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -12017,10 +12068,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="245" t="s">
+      <c r="S48" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="246"/>
+      <c r="T48" s="250"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -12173,11 +12224,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="279"/>
+      <c r="AQ49" s="282"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="239"/>
-      <c r="AV49" s="240"/>
+      <c r="AU49" s="243"/>
+      <c r="AV49" s="244"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -12189,11 +12240,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="279"/>
+      <c r="BK49" s="282"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="239"/>
-      <c r="BP49" s="240"/>
+      <c r="BO49" s="243"/>
+      <c r="BP49" s="244"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -12204,20 +12255,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="279"/>
+      <c r="CD49" s="282"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="239"/>
-      <c r="CI49" s="240"/>
+      <c r="CH49" s="243"/>
+      <c r="CI49" s="244"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="245" t="s">
+      <c r="AJ50" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="246"/>
+      <c r="AK50" s="250"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -12228,19 +12279,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="279"/>
+      <c r="AQ50" s="282"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="239"/>
-      <c r="AV50" s="240"/>
+      <c r="AU50" s="243"/>
+      <c r="AV50" s="244"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="245" t="s">
+      <c r="BD50" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="246"/>
+      <c r="BE50" s="250"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -12249,18 +12300,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="279"/>
+      <c r="BK50" s="282"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="239"/>
-      <c r="BP50" s="240"/>
+      <c r="BO50" s="243"/>
+      <c r="BP50" s="244"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="245" t="s">
+      <c r="BW50" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="246"/>
+      <c r="BX50" s="250"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -12269,21 +12320,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="279"/>
+      <c r="CD50" s="282"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="239"/>
-      <c r="CI50" s="240"/>
+      <c r="CH50" s="243"/>
+      <c r="CI50" s="244"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="247" t="s">
+      <c r="B51" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="248"/>
-      <c r="D51" s="249"/>
+      <c r="C51" s="252"/>
+      <c r="D51" s="253"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -12333,14 +12384,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="280"/>
+      <c r="AQ51" s="283"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="281"/>
-      <c r="AV51" s="274"/>
+      <c r="AU51" s="284"/>
+      <c r="AV51" s="285"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -12352,14 +12403,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="280"/>
+      <c r="BK51" s="283"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="281"/>
-      <c r="BP51" s="274"/>
+      <c r="BO51" s="284"/>
+      <c r="BP51" s="285"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -12370,14 +12421,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="280"/>
+      <c r="CD51" s="283"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="281"/>
-      <c r="CI51" s="274"/>
+      <c r="CH51" s="284"/>
+      <c r="CI51" s="285"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -12398,11 +12449,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="247" t="s">
+      <c r="V52" s="251" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="248"/>
-      <c r="X52" s="249"/>
+      <c r="W52" s="252"/>
+      <c r="X52" s="253"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -13492,10 +13543,10 @@
       </c>
     </row>
     <row r="66" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="245" t="s">
+      <c r="B66" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="246"/>
+      <c r="C66" s="250"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -13508,8 +13559,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="239"/>
-      <c r="O66" s="240"/>
+      <c r="N66" s="243"/>
+      <c r="O66" s="244"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -13536,18 +13587,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="238"/>
+      <c r="J67" s="242"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="239"/>
-      <c r="O67" s="240"/>
+      <c r="N67" s="243"/>
+      <c r="O67" s="244"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="245" t="s">
+      <c r="V67" s="249" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="246"/>
+      <c r="W67" s="250"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -13559,8 +13610,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="239"/>
-      <c r="AI67" s="240"/>
+      <c r="AH67" s="243"/>
+      <c r="AI67" s="244"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -13574,7 +13625,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="273"/>
+      <c r="J68" s="288"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -13590,10 +13641,10 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="238"/>
+      <c r="AD68" s="242"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="239"/>
-      <c r="AI68" s="240"/>
+      <c r="AH68" s="243"/>
+      <c r="AI68" s="244"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
@@ -13609,7 +13660,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="273"/>
+      <c r="AD69" s="288"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -13621,22 +13672,30 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -13652,30 +13711,22 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.4 _8:19PM
Rw Usage Updates S.1.0.0.4 _8:19PM
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.8.xlsx
+++ b/Usage_S_1.0.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6E984E-53B3-4175-B5F7-42C566809E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B36B633-FB68-4684-A7C2-484D22A48C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="226">
   <si>
     <t>UnSettled</t>
   </si>
@@ -896,7 +896,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -984,6 +984,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2197,6 +2203,9 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2233,6 +2242,39 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2269,46 +2311,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2322,22 +2334,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2627,7 +2635,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,15 +2672,15 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="247">
+      <c r="C2" s="248">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="251" t="s">
+      <c r="E2" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="252"/>
-      <c r="G2" s="253"/>
+      <c r="F2" s="253"/>
+      <c r="G2" s="254"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2721,19 +2729,19 @@
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="246" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="248"/>
+      <c r="C3" s="249"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="246"/>
+      <c r="A4" s="247"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -2901,7 +2909,7 @@
       <c r="E7" s="165">
         <v>10</v>
       </c>
-      <c r="F7" s="289">
+      <c r="F7" s="242">
         <v>10</v>
       </c>
       <c r="G7" s="127"/>
@@ -2950,7 +2958,7 @@
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="219"/>
-      <c r="F8" s="289">
+      <c r="F8" s="242">
         <v>35</v>
       </c>
       <c r="G8" s="190"/>
@@ -3058,6 +3066,9 @@
         <v>17</v>
       </c>
       <c r="J10" s="213"/>
+      <c r="K10" s="169" t="s">
+        <v>222</v>
+      </c>
       <c r="L10" s="83" t="s">
         <v>143</v>
       </c>
@@ -3097,7 +3108,7 @@
       <c r="E11" s="221">
         <v>5</v>
       </c>
-      <c r="F11" s="289">
+      <c r="F11" s="242">
         <v>15</v>
       </c>
       <c r="G11" s="184"/>
@@ -3211,8 +3222,8 @@
       <c r="J13" s="228" t="s">
         <v>186</v>
       </c>
-      <c r="K13" s="169" t="s">
-        <v>222</v>
+      <c r="K13" s="194" t="s">
+        <v>208</v>
       </c>
       <c r="L13" s="183" t="s">
         <v>155</v>
@@ -3235,6 +3246,9 @@
       <c r="R13"/>
       <c r="S13" s="154">
         <v>0.84375</v>
+      </c>
+      <c r="T13" s="290">
+        <v>1</v>
       </c>
       <c r="U13" s="24" t="s">
         <v>223</v>
@@ -3330,10 +3344,10 @@
     <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="249" t="s">
+      <c r="E17" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="250"/>
+      <c r="F17" s="251"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
@@ -3343,8 +3357,8 @@
       <c r="J17" s="119"/>
       <c r="K17" s="216"/>
       <c r="L17" s="119"/>
-      <c r="Q17" s="243"/>
-      <c r="R17" s="244"/>
+      <c r="Q17" s="244"/>
+      <c r="R17" s="245"/>
     </row>
     <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -3360,16 +3374,15 @@
       <c r="G18" s="20"/>
       <c r="I18" s="226"/>
       <c r="J18" s="119"/>
-      <c r="K18" s="216"/>
       <c r="L18" s="119"/>
-      <c r="M18" s="242"/>
-      <c r="Q18" s="243"/>
-      <c r="R18" s="244"/>
+      <c r="M18" s="243"/>
+      <c r="Q18" s="244"/>
+      <c r="R18" s="245"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="242"/>
+      <c r="M19" s="243"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="227"/>
@@ -3419,18 +3432,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="267" t="s">
+      <c r="E1" s="255" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="269"/>
+      <c r="F1" s="257"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="267" t="s">
+      <c r="H1" s="255" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="268"/>
-      <c r="J1" s="269"/>
+      <c r="I1" s="256"/>
+      <c r="J1" s="257"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3448,7 +3461,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="270">
+      <c r="B2" s="258">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -3475,15 +3488,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="273">
+      <c r="K2" s="261">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="264">
+      <c r="L2" s="276">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="254">
+      <c r="M2" s="266">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -3494,7 +3507,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="271"/>
+      <c r="B3" s="259"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3509,13 +3522,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="274"/>
-      <c r="L3" s="265"/>
-      <c r="M3" s="255"/>
+      <c r="K3" s="262"/>
+      <c r="L3" s="277"/>
+      <c r="M3" s="267"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="272"/>
+      <c r="B4" s="260"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3530,9 +3543,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="274"/>
-      <c r="L4" s="265"/>
-      <c r="M4" s="255"/>
+      <c r="K4" s="262"/>
+      <c r="L4" s="277"/>
+      <c r="M4" s="267"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -3614,7 +3627,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="256">
+      <c r="B7" s="268">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -3631,22 +3644,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="258">
+      <c r="K7" s="270">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="260">
+      <c r="L7" s="272">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="262">
+      <c r="M7" s="274">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="257"/>
+      <c r="B8" s="269"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -3667,9 +3680,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="259"/>
-      <c r="L8" s="261"/>
-      <c r="M8" s="263"/>
+      <c r="K8" s="271"/>
+      <c r="L8" s="273"/>
+      <c r="M8" s="275"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -3749,7 +3762,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="256">
+      <c r="B11" s="268">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3776,7 +3789,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="257"/>
+      <c r="B12" s="269"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3833,7 +3846,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="256">
+      <c r="B14" s="268">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3856,7 +3869,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="257"/>
+      <c r="B15" s="269"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3880,7 +3893,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="270">
+      <c r="B16" s="258">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3911,7 +3924,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="271"/>
+      <c r="B17" s="259"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3929,7 +3942,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="270">
+      <c r="B18" s="258">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3958,7 +3971,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="272"/>
+      <c r="B19" s="260"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4018,7 +4031,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="275">
+      <c r="B21" s="264">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4046,7 +4059,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="276"/>
+      <c r="B22" s="265"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4098,7 +4111,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="247">
+      <c r="B24" s="248">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -4127,7 +4140,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="248"/>
+      <c r="B25" s="249"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -4155,7 +4168,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="247">
+      <c r="B26" s="248">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -4186,7 +4199,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="266"/>
+      <c r="B27" s="263"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4217,7 +4230,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="247">
+      <c r="B28" s="248">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -4239,7 +4252,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="248"/>
+      <c r="B29" s="249"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -4265,7 +4278,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="247">
+      <c r="B30" s="248">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -4288,7 +4301,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="248"/>
+      <c r="B31" s="249"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4315,7 +4328,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="247">
+      <c r="B32" s="248">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -4337,7 +4350,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="248"/>
+      <c r="B33" s="249"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4390,7 +4403,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="247">
+      <c r="B35" s="248">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -4417,7 +4430,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="248"/>
+      <c r="B36" s="249"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -4439,7 +4452,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="247">
+      <c r="B37" s="248">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -4472,7 +4485,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="248"/>
+      <c r="B38" s="249"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -4490,7 +4503,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="247">
+      <c r="B39" s="248">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -4517,7 +4530,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="266"/>
+      <c r="B40" s="263"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -4545,7 +4558,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="247">
+      <c r="B41" s="248">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -4572,7 +4585,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="266"/>
+      <c r="B42" s="263"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -4590,7 +4603,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="248"/>
+      <c r="B43" s="249"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -4619,7 +4632,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="247">
+      <c r="B44" s="248">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -4645,7 +4658,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="248"/>
+      <c r="B45" s="249"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -4670,7 +4683,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="247">
+      <c r="B46" s="248">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -4692,7 +4705,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="266"/>
+      <c r="B47" s="263"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -4713,7 +4726,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="247">
+      <c r="B48" s="248">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -4733,7 +4746,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B49" s="266"/>
+      <c r="B49" s="263"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -4759,7 +4772,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="266"/>
+      <c r="B50" s="263"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -4786,7 +4799,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="247">
+      <c r="B51" s="248">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -4808,7 +4821,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="248"/>
+      <c r="B52" s="249"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -4835,7 +4848,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="247">
+      <c r="B53" s="248">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -4863,17 +4876,17 @@
       <c r="M53" s="18"/>
     </row>
     <row r="54" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="248"/>
+      <c r="B54" s="249"/>
       <c r="C54" s="142"/>
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
       <c r="F54" s="18"/>
-      <c r="G54" s="290">
+      <c r="G54" s="18">
         <v>60</v>
       </c>
       <c r="H54" s="18"/>
       <c r="I54" s="18"/>
-      <c r="J54" s="290">
+      <c r="J54" s="18">
         <v>20</v>
       </c>
       <c r="K54" s="18"/>
@@ -4882,6 +4895,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="M2:M4"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B2:B4"/>
@@ -4898,19 +4924,6 @@
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="M2:M4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L2:L4"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B44:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8117,10 +8130,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="249" t="s">
+      <c r="AG24" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="250"/>
+      <c r="AH24" s="251"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -8140,10 +8153,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="249" t="s">
+      <c r="AZ24" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="250"/>
+      <c r="BA24" s="251"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -8163,10 +8176,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="249" t="s">
+      <c r="BR24" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="250"/>
+      <c r="BS24" s="251"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -8189,10 +8202,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="251" t="s">
+      <c r="B26" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="253"/>
+      <c r="C26" s="254"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8229,10 +8242,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="251" t="s">
+      <c r="R26" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="253"/>
+      <c r="S26" s="254"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8269,10 +8282,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="251" t="s">
+      <c r="AG26" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="253"/>
+      <c r="AH26" s="254"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8309,10 +8322,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="251" t="s">
+      <c r="AW26" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="253"/>
+      <c r="AX26" s="254"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8349,10 +8362,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="251" t="s">
+      <c r="BM26" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="253"/>
+      <c r="BN26" s="254"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9346,7 +9359,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="277">
+      <c r="AX32" s="287">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -9384,7 +9397,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="277">
+      <c r="BN32" s="287">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -9533,7 +9546,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="278"/>
+      <c r="AX33" s="288"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9569,7 +9582,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="278"/>
+      <c r="BN33" s="288"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9720,7 +9733,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="279"/>
+      <c r="AX34" s="289"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9758,7 +9771,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="279"/>
+      <c r="BN34" s="289"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9989,10 +10002,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="249" t="s">
+      <c r="B36" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="250"/>
+      <c r="C36" s="251"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -10010,10 +10023,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="249" t="s">
+      <c r="R36" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="250"/>
+      <c r="S36" s="251"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -10031,10 +10044,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="249" t="s">
+      <c r="AG36" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="250"/>
+      <c r="AH36" s="251"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -10052,10 +10065,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="249" t="s">
+      <c r="AW36" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="250"/>
+      <c r="AX36" s="251"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -10073,10 +10086,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="249" t="s">
+      <c r="BM36" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="250"/>
+      <c r="BN36" s="251"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -10096,10 +10109,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="251" t="s">
+      <c r="B38" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="253"/>
+      <c r="C38" s="254"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10139,10 +10152,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="251" t="s">
+      <c r="S38" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="253"/>
+      <c r="T38" s="254"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10182,11 +10195,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="251" t="s">
+      <c r="AJ38" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="252"/>
-      <c r="AL38" s="253"/>
+      <c r="AK38" s="253"/>
+      <c r="AL38" s="254"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10231,11 +10244,11 @@
         <f ca="1">TODAY()</f>
         <v>45290</v>
       </c>
-      <c r="BD38" s="251" t="s">
+      <c r="BD38" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="252"/>
-      <c r="BF38" s="253"/>
+      <c r="BE38" s="253"/>
+      <c r="BF38" s="254"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10275,11 +10288,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="251" t="s">
+      <c r="BW38" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="252"/>
-      <c r="BY38" s="253"/>
+      <c r="BX38" s="253"/>
+      <c r="BY38" s="254"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11231,7 +11244,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="277">
+      <c r="C44" s="287">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -11269,10 +11282,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="286">
+      <c r="S44" s="280">
         <v>25</v>
       </c>
-      <c r="T44" s="277">
+      <c r="T44" s="287">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -11281,7 +11294,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="280" t="s">
+      <c r="W44" s="282" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -11310,10 +11323,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="286">
+      <c r="AJ44" s="280">
         <v>50</v>
       </c>
-      <c r="AK44" s="277">
+      <c r="AK44" s="287">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -11323,7 +11336,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="280" t="s">
+      <c r="AO44" s="282" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -11353,7 +11366,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="286">
+      <c r="BD44" s="280">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -11364,7 +11377,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="280" t="s">
+      <c r="BI44" s="282" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -11393,7 +11406,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="286">
+      <c r="BW44" s="280">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -11404,7 +11417,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="280" t="s">
+      <c r="CB44" s="282" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -11436,7 +11449,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="278"/>
+      <c r="C45" s="288"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -11470,15 +11483,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="287"/>
-      <c r="T45" s="279"/>
+      <c r="S45" s="281"/>
+      <c r="T45" s="289"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="281"/>
+      <c r="W45" s="283"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11505,8 +11518,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="287"/>
-      <c r="AK45" s="279"/>
+      <c r="AJ45" s="281"/>
+      <c r="AK45" s="289"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -11514,7 +11527,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="281"/>
+      <c r="AO45" s="283"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11542,7 +11555,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="287"/>
+      <c r="BD45" s="281"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -11553,7 +11566,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="281"/>
+      <c r="BI45" s="283"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11580,7 +11593,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="287"/>
+      <c r="BW45" s="281"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -11589,7 +11602,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="281"/>
+      <c r="CB45" s="283"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11619,7 +11632,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="279"/>
+      <c r="C46" s="289"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -12046,10 +12059,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="249" t="s">
+      <c r="B48" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="250"/>
+      <c r="C48" s="251"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -12068,10 +12081,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="249" t="s">
+      <c r="S48" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="250"/>
+      <c r="T48" s="251"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -12224,11 +12237,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="282"/>
+      <c r="AQ49" s="284"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="243"/>
-      <c r="AV49" s="244"/>
+      <c r="AU49" s="244"/>
+      <c r="AV49" s="245"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -12240,11 +12253,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="282"/>
+      <c r="BK49" s="284"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="243"/>
-      <c r="BP49" s="244"/>
+      <c r="BO49" s="244"/>
+      <c r="BP49" s="245"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -12255,20 +12268,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="282"/>
+      <c r="CD49" s="284"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="243"/>
-      <c r="CI49" s="244"/>
+      <c r="CH49" s="244"/>
+      <c r="CI49" s="245"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="249" t="s">
+      <c r="AJ50" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="250"/>
+      <c r="AK50" s="251"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -12279,19 +12292,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="282"/>
+      <c r="AQ50" s="284"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="243"/>
-      <c r="AV50" s="244"/>
+      <c r="AU50" s="244"/>
+      <c r="AV50" s="245"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="249" t="s">
+      <c r="BD50" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="250"/>
+      <c r="BE50" s="251"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -12300,18 +12313,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="282"/>
+      <c r="BK50" s="284"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="243"/>
-      <c r="BP50" s="244"/>
+      <c r="BO50" s="244"/>
+      <c r="BP50" s="245"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="249" t="s">
+      <c r="BW50" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="250"/>
+      <c r="BX50" s="251"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -12320,21 +12333,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="282"/>
+      <c r="CD50" s="284"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="243"/>
-      <c r="CI50" s="244"/>
+      <c r="CH50" s="244"/>
+      <c r="CI50" s="245"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="251" t="s">
+      <c r="B51" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="252"/>
-      <c r="D51" s="253"/>
+      <c r="C51" s="253"/>
+      <c r="D51" s="254"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -12384,14 +12397,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="283"/>
+      <c r="AQ51" s="285"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="284"/>
-      <c r="AV51" s="285"/>
+      <c r="AU51" s="286"/>
+      <c r="AV51" s="279"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -12403,14 +12416,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="283"/>
+      <c r="BK51" s="285"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="284"/>
-      <c r="BP51" s="285"/>
+      <c r="BO51" s="286"/>
+      <c r="BP51" s="279"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -12421,14 +12434,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="283"/>
+      <c r="CD51" s="285"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="284"/>
-      <c r="CI51" s="285"/>
+      <c r="CH51" s="286"/>
+      <c r="CI51" s="279"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -12449,11 +12462,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="251" t="s">
+      <c r="V52" s="252" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="252"/>
-      <c r="X52" s="253"/>
+      <c r="W52" s="253"/>
+      <c r="X52" s="254"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -13543,10 +13556,10 @@
       </c>
     </row>
     <row r="66" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="249" t="s">
+      <c r="B66" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="250"/>
+      <c r="C66" s="251"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -13559,8 +13572,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="243"/>
-      <c r="O66" s="244"/>
+      <c r="N66" s="244"/>
+      <c r="O66" s="245"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -13587,18 +13600,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="242"/>
+      <c r="J67" s="243"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="243"/>
-      <c r="O67" s="244"/>
+      <c r="N67" s="244"/>
+      <c r="O67" s="245"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="249" t="s">
+      <c r="V67" s="250" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="250"/>
+      <c r="W67" s="251"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -13610,8 +13623,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="243"/>
-      <c r="AI67" s="244"/>
+      <c r="AH67" s="244"/>
+      <c r="AI67" s="245"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -13625,7 +13638,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="288"/>
+      <c r="J68" s="278"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -13641,10 +13654,10 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="242"/>
+      <c r="AD68" s="243"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="243"/>
-      <c r="AI68" s="244"/>
+      <c r="AH68" s="244"/>
+      <c r="AI68" s="245"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
@@ -13660,7 +13673,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="288"/>
+      <c r="AD69" s="278"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -13672,30 +13685,22 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -13711,22 +13716,30 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Rw Usage Updates S.1.0.0.7 _12:00PM
Boat Enabled -
InCapacity - [0] , NodeW - [-3] , BirdW - [6] , FuelW - [20] , OnHost - [8+1]
VillageW=[1] , [X-MarketShieldMatrix-X] = [1,20,30,2]
Rw - Local(Left Running With Cost ) - [For Business/Shop/Market only] -
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.8.xlsx
+++ b/Usage_S_1.0.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247007C7-BB1B-4D37-8AC3-05C0AB774B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450517AA-FCBD-4DF1-91E2-C0F288660208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2103" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2232" uniqueCount="244">
   <si>
     <t>UnSettled</t>
   </si>
@@ -720,6 +720,54 @@
   </si>
   <si>
     <t>X-VillageW(ChannaGhara) - X</t>
+  </si>
+  <si>
+    <t>X-Biju Aadarsha Colony - X</t>
+  </si>
+  <si>
+    <t>X-LaxmiNarayan Lane- X</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>X-Durga Market- X</t>
+  </si>
+  <si>
+    <t>X-GH School Road- X</t>
+  </si>
+  <si>
+    <t>X-Accounts Colony- X</t>
+  </si>
+  <si>
+    <t>X-Hata Bazar- X</t>
+  </si>
+  <si>
+    <t>WR</t>
+  </si>
+  <si>
+    <t>X-Kudiary Bazar- X</t>
+  </si>
+  <si>
+    <t>X-MG Square- X</t>
+  </si>
+  <si>
+    <t>X-NuaGaon- X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area MatriX </t>
+  </si>
+  <si>
+    <t>X-RC Colony- X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Shield MatriX </t>
+  </si>
+  <si>
+    <t>X-MSM-X</t>
   </si>
 </sst>
 </file>
@@ -1638,7 +1686,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="297">
+  <cellXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2237,6 +2285,12 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2273,6 +2327,42 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2306,52 +2396,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2365,22 +2416,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2668,10 +2778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:AI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AG6" sqref="AG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2698,25 +2808,51 @@
     <col min="21" max="21" width="11.140625" style="24" customWidth="1"/>
     <col min="22" max="22" width="5.140625" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="3.85546875" customWidth="1"/>
+    <col min="29" max="30" width="5.28515625" customWidth="1"/>
+    <col min="31" max="31" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z1" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="AA1" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB1" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC1" s="315" t="s">
+        <v>236</v>
+      </c>
+      <c r="AD1" s="314" t="s">
+        <v>224</v>
+      </c>
+      <c r="AF1" s="318" t="s">
+        <v>242</v>
+      </c>
+      <c r="AG1" s="319"/>
+      <c r="AH1" s="319"/>
+      <c r="AI1" s="320"/>
+    </row>
+    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="251">
+      <c r="C2" s="253">
         <f>B3+B4</f>
         <v>0</v>
       </c>
-      <c r="E2" s="255" t="s">
+      <c r="E2" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="256"/>
-      <c r="G2" s="257"/>
+      <c r="F2" s="258"/>
+      <c r="G2" s="259"/>
       <c r="H2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2761,23 +2897,48 @@
       </c>
       <c r="W2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
+      </c>
+      <c r="AA2" s="26">
+        <f>SUM(AA3:AA17)</f>
+        <v>1</v>
+      </c>
+      <c r="AB2" s="26">
+        <f>SUM(AB3:AB17)</f>
+        <v>20</v>
+      </c>
+      <c r="AC2" s="8">
+        <f>SUM(AC3:AC17)</f>
+        <v>30</v>
+      </c>
+      <c r="AD2" s="8">
+        <f>SUM(AD3:AD17)</f>
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="249" t="s">
+    <row r="3" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="251" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34">
         <v>0</v>
       </c>
-      <c r="C3" s="252"/>
+      <c r="C3" s="254"/>
       <c r="D3" s="162" t="s">
         <v>36</v>
       </c>
+      <c r="Z3" s="169" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA3" s="316"/>
+      <c r="AB3" s="316"/>
+      <c r="AC3" s="43">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="44"/>
     </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="250"/>
+    <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="252"/>
       <c r="B4" s="34">
         <v>0</v>
       </c>
@@ -2785,12 +2946,10 @@
         <v>35</v>
       </c>
       <c r="E4" s="244">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F4" s="205"/>
-      <c r="G4" s="296">
-        <v>20</v>
-      </c>
+      <c r="G4" s="247"/>
       <c r="H4" s="9" t="s">
         <v>199</v>
       </c>
@@ -2819,30 +2978,35 @@
         <v>30</v>
       </c>
       <c r="Q4" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="S4" s="154">
-        <v>0.88611111111111107</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="T4" s="240">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U4" s="245">
         <v>45292</v>
       </c>
+      <c r="Z4" s="169" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA4" s="298"/>
+      <c r="AB4" s="298"/>
+      <c r="AC4" s="297">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="49"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="D5" s="156">
         <v>-2</v>
       </c>
-      <c r="E5" s="218">
-        <v>5</v>
-      </c>
+      <c r="E5" s="218"/>
       <c r="F5" s="206"/>
-      <c r="G5" s="37">
-        <v>20</v>
-      </c>
+      <c r="G5" s="37"/>
       <c r="H5" s="9" t="s">
         <v>1</v>
       </c>
@@ -2852,9 +3016,7 @@
       <c r="J5" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K5" s="215" t="s">
-        <v>218</v>
-      </c>
+      <c r="K5" s="215"/>
       <c r="L5" s="167" t="s">
         <v>142</v>
       </c>
@@ -2882,21 +3044,26 @@
       <c r="U5" s="245">
         <v>45292</v>
       </c>
+      <c r="Z5" s="215" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA5" s="298"/>
+      <c r="AB5" s="298"/>
+      <c r="AC5" s="297">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="49"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
-        <v>2887</v>
+        <v>2932</v>
       </c>
       <c r="C6">
-        <v>6078</v>
-      </c>
-      <c r="E6" s="218">
-        <v>5</v>
-      </c>
+        <v>6033</v>
+      </c>
+      <c r="E6" s="218"/>
       <c r="F6" s="207"/>
-      <c r="G6" s="127">
-        <v>40</v>
-      </c>
+      <c r="G6" s="127"/>
       <c r="H6" s="9" t="s">
         <v>203</v>
       </c>
@@ -2906,9 +3073,7 @@
       <c r="J6" s="213" t="s">
         <v>165</v>
       </c>
-      <c r="K6" s="169" t="s">
-        <v>220</v>
-      </c>
+      <c r="K6" s="169"/>
       <c r="L6" s="83" t="s">
         <v>123</v>
       </c>
@@ -2936,21 +3101,26 @@
       <c r="U6" s="245">
         <v>45292</v>
       </c>
+      <c r="Z6" s="169" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA6" s="298"/>
+      <c r="AB6" s="26">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="297"/>
+      <c r="AD6" s="49"/>
     </row>
-    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="165">
-        <v>10</v>
-      </c>
+      <c r="E7" s="165"/>
       <c r="F7" s="242"/>
-      <c r="G7" s="177">
-        <v>10</v>
-      </c>
+      <c r="G7" s="177"/>
       <c r="H7" s="9" t="s">
         <v>188</v>
       </c>
@@ -2960,9 +3130,7 @@
       <c r="J7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="215" t="s">
-        <v>219</v>
-      </c>
+      <c r="K7" s="215"/>
       <c r="L7" s="83" t="s">
         <v>139</v>
       </c>
@@ -2993,10 +3161,23 @@
       <c r="U7" s="245">
         <v>45292</v>
       </c>
+      <c r="Z7" s="169" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA7" s="26">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="26">
+        <v>6</v>
+      </c>
+      <c r="AC7" s="297">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="49"/>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="219">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="F8" s="242"/>
       <c r="G8" s="190"/>
@@ -3026,29 +3207,38 @@
         <v>65</v>
       </c>
       <c r="Q8" s="154">
-        <v>0.57638888888888895</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="S8" s="154">
-        <v>0.57638888888888895</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="T8" s="240">
         <v>3</v>
       </c>
       <c r="U8" s="245">
-        <v>45292</v>
-      </c>
+        <v>45293</v>
+      </c>
+      <c r="Z8" s="169" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA8" s="298"/>
+      <c r="AB8" s="26">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="297">
+        <v>4</v>
+      </c>
+      <c r="AD8" s="49"/>
     </row>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8">
         <f>7000+B6+B5-C2</f>
-        <v>9887</v>
-      </c>
-      <c r="E9" s="163">
-        <v>14</v>
-      </c>
+        <v>9932</v>
+      </c>
+      <c r="E9" s="163"/>
       <c r="F9" s="165"/>
       <c r="G9" s="177"/>
       <c r="H9" s="9" t="s">
@@ -3090,15 +3280,20 @@
       <c r="U9" s="245">
         <v>45292</v>
       </c>
+      <c r="Z9" s="169" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA9" s="298"/>
+      <c r="AB9" s="312">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="297"/>
+      <c r="AD9" s="49"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="220">
-        <v>70</v>
-      </c>
+    <row r="10" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="220"/>
       <c r="F10" s="206"/>
-      <c r="G10" s="177">
-        <v>7</v>
-      </c>
+      <c r="G10" s="177"/>
       <c r="H10" s="9" t="s">
         <v>81</v>
       </c>
@@ -3136,8 +3331,19 @@
       <c r="U10" s="245">
         <v>45292</v>
       </c>
+      <c r="Z10" s="169" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA10" s="297"/>
+      <c r="AB10" s="312">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="297"/>
+      <c r="AD10" s="49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -3146,14 +3352,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="221">
-        <v>5</v>
-      </c>
-      <c r="F11" s="242">
-        <v>20</v>
-      </c>
-      <c r="G11" s="37">
         <v>10</v>
       </c>
+      <c r="F11" s="242"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="9" t="s">
         <v>102</v>
       </c>
@@ -3164,7 +3366,7 @@
         <v>116</v>
       </c>
       <c r="K11" s="194" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="L11" s="83" t="s">
         <v>124</v>
@@ -3196,15 +3398,22 @@
       <c r="U11" s="245">
         <v>45292</v>
       </c>
+      <c r="Z11" s="169" t="s">
+        <v>233</v>
+      </c>
+      <c r="AA11" s="297"/>
+      <c r="AB11" s="312">
+        <v>2</v>
+      </c>
+      <c r="AC11" s="297">
+        <v>5</v>
+      </c>
+      <c r="AD11" s="49"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="165">
-        <v>10</v>
-      </c>
+    <row r="12" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="165"/>
       <c r="F12" s="205"/>
-      <c r="G12" s="164">
-        <v>200</v>
-      </c>
+      <c r="G12" s="164"/>
       <c r="H12" s="28" t="s">
         <v>128</v>
       </c>
@@ -3212,9 +3421,7 @@
         <v>17</v>
       </c>
       <c r="J12" s="213"/>
-      <c r="K12" s="169" t="s">
-        <v>221</v>
-      </c>
+      <c r="K12" s="169"/>
       <c r="L12" s="224" t="s">
         <v>123</v>
       </c>
@@ -3243,22 +3450,27 @@
       <c r="U12" s="245">
         <v>45292</v>
       </c>
+      <c r="Z12" s="169" t="s">
+        <v>234</v>
+      </c>
+      <c r="AA12" s="297"/>
+      <c r="AB12" s="312">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="297"/>
+      <c r="AD12" s="49"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>9887</v>
-      </c>
-      <c r="E13" s="36">
-        <v>1</v>
-      </c>
+        <v>9932</v>
+      </c>
+      <c r="E13" s="36"/>
       <c r="F13" s="206"/>
-      <c r="G13" s="295">
-        <v>25</v>
-      </c>
+      <c r="G13" s="246"/>
       <c r="H13" s="9" t="s">
         <v>189</v>
       </c>
@@ -3268,9 +3480,7 @@
       <c r="J13" s="228" t="s">
         <v>186</v>
       </c>
-      <c r="K13" s="194" t="s">
-        <v>208</v>
-      </c>
+      <c r="K13" s="194"/>
       <c r="L13" s="183" t="s">
         <v>155</v>
       </c>
@@ -3299,13 +3509,22 @@
       <c r="U13" s="245">
         <v>45292</v>
       </c>
+      <c r="Z13" s="169" t="s">
+        <v>235</v>
+      </c>
+      <c r="AA13" s="297"/>
+      <c r="AB13" s="312">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="297"/>
+      <c r="AD13" s="49">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
-      <c r="E14" s="165">
-        <v>10</v>
-      </c>
+      <c r="E14" s="165"/>
       <c r="F14" s="205"/>
       <c r="G14" s="184"/>
       <c r="H14" s="9" t="s">
@@ -3315,9 +3534,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="213"/>
-      <c r="K14" s="169" t="s">
-        <v>227</v>
-      </c>
+      <c r="K14" s="169"/>
       <c r="L14" s="83" t="s">
         <v>124</v>
       </c>
@@ -3339,8 +3556,15 @@
       <c r="U14" s="245">
         <v>45292</v>
       </c>
+      <c r="Z14" s="169" t="s">
+        <v>237</v>
+      </c>
+      <c r="AA14" s="297"/>
+      <c r="AB14" s="297"/>
+      <c r="AC14" s="297"/>
+      <c r="AD14" s="49"/>
     </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>2</v>
       </c>
@@ -3378,35 +3602,62 @@
       <c r="U15" s="245">
         <v>45292</v>
       </c>
+      <c r="Z15" s="169" t="s">
+        <v>238</v>
+      </c>
+      <c r="AA15" s="297"/>
+      <c r="AB15" s="313"/>
+      <c r="AC15" s="297">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="49"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="I16" s="234"/>
       <c r="J16" s="119"/>
       <c r="K16" s="216"/>
       <c r="L16" s="119"/>
+      <c r="Z16" s="169" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA16" s="297"/>
+      <c r="AB16" s="297"/>
+      <c r="AC16" s="297">
+        <v>4</v>
+      </c>
+      <c r="AD16" s="49"/>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
-      <c r="E17" s="253" t="s">
+      <c r="E17" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="254"/>
+      <c r="F17" s="256"/>
       <c r="G17" s="189"/>
       <c r="H17" s="9">
         <f>SUM(E4:G15)</f>
-        <v>562</v>
+        <v>45</v>
       </c>
       <c r="I17" s="26"/>
       <c r="J17" s="119"/>
       <c r="K17" s="216"/>
       <c r="L17" s="119"/>
-      <c r="Q17" s="247"/>
-      <c r="R17" s="248"/>
+      <c r="Q17" s="249"/>
+      <c r="R17" s="250"/>
+      <c r="Z17" s="169" t="s">
+        <v>241</v>
+      </c>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="312">
+        <v>2</v>
+      </c>
+      <c r="AC17" s="50"/>
+      <c r="AD17" s="51"/>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>0</v>
       </c>
@@ -3421,21 +3672,22 @@
       <c r="I18" s="226"/>
       <c r="J18" s="119"/>
       <c r="L18" s="119"/>
-      <c r="M18" s="246"/>
-      <c r="Q18" s="247"/>
-      <c r="R18" s="248"/>
+      <c r="M18" s="248"/>
+      <c r="Q18" s="249"/>
+      <c r="R18" s="250"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="I19" s="226"/>
       <c r="L19" s="119"/>
-      <c r="M19" s="246"/>
+      <c r="M19" s="248"/>
     </row>
-    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="227"/>
       <c r="L20" s="119"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="M18:M19"/>
     <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="R17:R18"/>
@@ -3451,10 +3703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:T56"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3478,18 +3730,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="259" t="s">
+      <c r="E1" s="273" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="261"/>
+      <c r="F1" s="275"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="259" t="s">
+      <c r="H1" s="273" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="260"/>
-      <c r="J1" s="261"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="275"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -3507,7 +3759,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="262">
+      <c r="B2" s="276">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -3534,26 +3786,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="265">
+      <c r="K2" s="279">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="279">
+      <c r="L2" s="270">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="269">
+      <c r="M2" s="260">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J56)</f>
-        <v>9847</v>
+        <f>SUM(E2:J57)</f>
+        <v>9892</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="263"/>
+      <c r="B3" s="277"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -3568,13 +3820,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="266"/>
-      <c r="L3" s="280"/>
-      <c r="M3" s="270"/>
+      <c r="K3" s="280"/>
+      <c r="L3" s="271"/>
+      <c r="M3" s="261"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="264"/>
+      <c r="B4" s="278"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -3589,9 +3841,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="266"/>
-      <c r="L4" s="280"/>
-      <c r="M4" s="270"/>
+      <c r="K4" s="280"/>
+      <c r="L4" s="271"/>
+      <c r="M4" s="261"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -3673,7 +3925,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="271">
+      <c r="B7" s="262">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -3690,22 +3942,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="273">
+      <c r="K7" s="264">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="275">
+      <c r="L7" s="266">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="277">
+      <c r="M7" s="268">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="272"/>
+      <c r="B8" s="263"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -3726,9 +3978,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="274"/>
-      <c r="L8" s="276"/>
-      <c r="M8" s="278"/>
+      <c r="K8" s="265"/>
+      <c r="L8" s="267"/>
+      <c r="M8" s="269"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -3808,7 +4060,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="271">
+      <c r="B11" s="262">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3835,7 +4087,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="272"/>
+      <c r="B12" s="263"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3892,7 +4144,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="271">
+      <c r="B14" s="262">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3915,7 +4167,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="272"/>
+      <c r="B15" s="263"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3939,7 +4191,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="262">
+      <c r="B16" s="276">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3970,7 +4222,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="263"/>
+      <c r="B17" s="277"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3988,7 +4240,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="262">
+      <c r="B18" s="276">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -4017,7 +4269,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="264"/>
+      <c r="B19" s="278"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -4077,7 +4329,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="267">
+      <c r="B21" s="281">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -4105,7 +4357,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="268"/>
+      <c r="B22" s="282"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -4157,7 +4409,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="251">
+      <c r="B24" s="253">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -4186,7 +4438,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="252"/>
+      <c r="B25" s="254"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -4214,7 +4466,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="251">
+      <c r="B26" s="253">
         <v>17</v>
       </c>
       <c r="C26" s="161"/>
@@ -4245,7 +4497,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="258"/>
+      <c r="B27" s="272"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -4276,7 +4528,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="251">
+      <c r="B28" s="253">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -4298,7 +4550,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="252"/>
+      <c r="B29" s="254"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -4324,7 +4576,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="251">
+      <c r="B30" s="253">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -4347,7 +4599,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="252"/>
+      <c r="B31" s="254"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4374,7 +4626,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="251">
+      <c r="B32" s="253">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -4396,7 +4648,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="252"/>
+      <c r="B33" s="254"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4449,7 +4701,7 @@
       <c r="M34" s="82"/>
     </row>
     <row r="35" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="251">
+      <c r="B35" s="253">
         <v>22</v>
       </c>
       <c r="C35" s="96"/>
@@ -4476,7 +4728,7 @@
       <c r="A36" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="252"/>
+      <c r="B36" s="254"/>
       <c r="C36" s="142"/>
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
@@ -4498,7 +4750,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="251">
+      <c r="B37" s="253">
         <v>23</v>
       </c>
       <c r="C37" s="142"/>
@@ -4531,7 +4783,7 @@
       <c r="A38" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="252"/>
+      <c r="B38" s="254"/>
       <c r="C38" s="96"/>
       <c r="D38" s="82"/>
       <c r="E38" s="82"/>
@@ -4549,7 +4801,7 @@
       <c r="M38" s="82"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="251">
+      <c r="B39" s="253">
         <v>24</v>
       </c>
       <c r="C39" s="142"/>
@@ -4576,7 +4828,7 @@
       <c r="A40" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="258"/>
+      <c r="B40" s="272"/>
       <c r="C40" s="96"/>
       <c r="D40" s="82">
         <v>210</v>
@@ -4604,7 +4856,7 @@
       <c r="M40" s="82"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="251">
+      <c r="B41" s="253">
         <v>25</v>
       </c>
       <c r="C41" s="142"/>
@@ -4631,7 +4883,7 @@
       <c r="A42" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="258"/>
+      <c r="B42" s="272"/>
       <c r="C42" s="142"/>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
@@ -4649,7 +4901,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="252"/>
+      <c r="B43" s="254"/>
       <c r="C43" s="142"/>
       <c r="D43" s="18">
         <v>190</v>
@@ -4678,7 +4930,7 @@
       <c r="A44" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="251">
+      <c r="B44" s="253">
         <v>26</v>
       </c>
       <c r="C44" s="142"/>
@@ -4704,7 +4956,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="252"/>
+      <c r="B45" s="254"/>
       <c r="C45" s="142"/>
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
@@ -4729,7 +4981,7 @@
       <c r="A46" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="251">
+      <c r="B46" s="253">
         <v>27</v>
       </c>
       <c r="C46" s="142"/>
@@ -4751,7 +5003,7 @@
       <c r="M46" s="18"/>
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="258"/>
+      <c r="B47" s="272"/>
       <c r="C47" s="211"/>
       <c r="D47" s="132"/>
       <c r="E47" s="132"/>
@@ -4772,7 +5024,7 @@
       <c r="A48" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="251">
+      <c r="B48" s="253">
         <v>28</v>
       </c>
       <c r="C48" s="142"/>
@@ -4792,7 +5044,7 @@
       <c r="M48" s="18"/>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B49" s="258"/>
+      <c r="B49" s="272"/>
       <c r="C49" s="142"/>
       <c r="D49" s="18">
         <v>175</v>
@@ -4818,7 +5070,7 @@
       <c r="M49" s="18"/>
     </row>
     <row r="50" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="258"/>
+      <c r="B50" s="272"/>
       <c r="C50" s="96"/>
       <c r="D50" s="82"/>
       <c r="E50" s="82"/>
@@ -4845,7 +5097,7 @@
       <c r="A51" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B51" s="251">
+      <c r="B51" s="253">
         <v>29</v>
       </c>
       <c r="C51" s="142"/>
@@ -4867,7 +5119,7 @@
       <c r="M51" s="18"/>
     </row>
     <row r="52" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="252"/>
+      <c r="B52" s="254"/>
       <c r="C52" s="142"/>
       <c r="D52" s="18">
         <v>190</v>
@@ -4900,7 +5152,7 @@
       <c r="A53" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="251">
+      <c r="B53" s="253">
         <v>30</v>
       </c>
       <c r="C53" s="142"/>
@@ -4927,14 +5179,10 @@
       <c r="L53" s="18"/>
       <c r="M53" s="18"/>
       <c r="O53" s="48"/>
-      <c r="P53" s="294"/>
-      <c r="Q53" s="294"/>
-      <c r="R53" s="294"/>
-      <c r="S53" s="294"/>
       <c r="T53" s="49"/>
     </row>
     <row r="54" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="258"/>
+      <c r="B54" s="272"/>
       <c r="C54" s="96"/>
       <c r="D54" s="82"/>
       <c r="E54" s="82"/>
@@ -4961,7 +5209,7 @@
       <c r="A55" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="251">
+      <c r="B55" s="253">
         <v>31</v>
       </c>
       <c r="C55" s="96"/>
@@ -4988,34 +5236,69 @@
       <c r="L55" s="82"/>
       <c r="M55" s="82"/>
     </row>
-    <row r="56" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="252"/>
-      <c r="C56" s="142"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="272"/>
+      <c r="C56" s="96"/>
+      <c r="D56" s="82"/>
+      <c r="E56" s="82">
         <v>200</v>
       </c>
-      <c r="F56" s="18">
+      <c r="F56" s="82">
         <v>40</v>
       </c>
-      <c r="G56" s="293">
+      <c r="G56" s="82">
         <v>25</v>
       </c>
-      <c r="H56" s="293">
+      <c r="H56" s="82">
         <v>20</v>
       </c>
-      <c r="I56" s="293">
-        <v>17</v>
-      </c>
-      <c r="J56" s="293">
+      <c r="I56" s="82">
+        <v>17</v>
+      </c>
+      <c r="J56" s="82">
         <v>30</v>
       </c>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18"/>
-      <c r="M56" s="18"/>
+      <c r="K56" s="82"/>
+      <c r="L56" s="82"/>
+      <c r="M56" s="82"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="17">
+        <v>1</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="317">
+        <v>25</v>
+      </c>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="317">
+        <v>20</v>
+      </c>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B51:B52"/>
@@ -5031,21 +5314,6 @@
     <mergeCell ref="B46:B47"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="B53:B54"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B35:B36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5055,8 +5323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
   <dimension ref="A1:CL71"/>
   <sheetViews>
-    <sheetView topLeftCell="AM52" workbookViewId="0">
-      <selection activeCell="BA68" sqref="BA68:BA69"/>
+    <sheetView topLeftCell="BG52" workbookViewId="0">
+      <selection activeCell="BH59" sqref="BH59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6606,7 +6874,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -6651,7 +6919,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -6696,7 +6964,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
       </c>
       <c r="BR14" s="158" t="s">
         <v>44</v>
@@ -6741,7 +7009,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8252,10 +8520,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="253" t="s">
+      <c r="AG24" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="254"/>
+      <c r="AH24" s="256"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -8275,10 +8543,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="253" t="s">
+      <c r="AZ24" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="254"/>
+      <c r="BA24" s="256"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -8298,10 +8566,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="253" t="s">
+      <c r="BR24" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="254"/>
+      <c r="BS24" s="256"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -8324,10 +8592,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="255" t="s">
+      <c r="B26" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="257"/>
+      <c r="C26" s="259"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8364,10 +8632,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="255" t="s">
+      <c r="R26" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="257"/>
+      <c r="S26" s="259"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8404,10 +8672,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="255" t="s">
+      <c r="AG26" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="257"/>
+      <c r="AH26" s="259"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8444,10 +8712,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="255" t="s">
+      <c r="AW26" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="257"/>
+      <c r="AX26" s="259"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -8484,10 +8752,10 @@
       <c r="BJ26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="BM26" s="255" t="s">
+      <c r="BM26" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="BN26" s="257"/>
+      <c r="BN26" s="259"/>
       <c r="BO26" s="26" t="s">
         <v>43</v>
       </c>
@@ -9481,7 +9749,7 @@
       <c r="AW32" s="163">
         <v>25</v>
       </c>
-      <c r="AX32" s="290">
+      <c r="AX32" s="283">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -9519,7 +9787,7 @@
       <c r="BM32" s="163">
         <v>50</v>
       </c>
-      <c r="BN32" s="290">
+      <c r="BN32" s="283">
         <v>20</v>
       </c>
       <c r="BO32" s="9" t="s">
@@ -9668,7 +9936,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="163"/>
-      <c r="AX33" s="291"/>
+      <c r="AX33" s="284"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9704,7 +9972,7 @@
       <c r="BM33" s="140">
         <v>10</v>
       </c>
-      <c r="BN33" s="291"/>
+      <c r="BN33" s="284"/>
       <c r="BO33" s="9" t="s">
         <v>71</v>
       </c>
@@ -9855,7 +10123,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="292"/>
+      <c r="AX34" s="285"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -9893,7 +10161,7 @@
       <c r="BM34" s="165">
         <v>70</v>
       </c>
-      <c r="BN34" s="292"/>
+      <c r="BN34" s="285"/>
       <c r="BO34" s="9" t="s">
         <v>81</v>
       </c>
@@ -10124,10 +10392,10 @@
       </c>
     </row>
     <row r="36" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="253" t="s">
+      <c r="B36" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="254"/>
+      <c r="C36" s="256"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -10145,10 +10413,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="253" t="s">
+      <c r="R36" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="254"/>
+      <c r="S36" s="256"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -10166,10 +10434,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="253" t="s">
+      <c r="AG36" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="254"/>
+      <c r="AH36" s="256"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -10187,10 +10455,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="253" t="s">
+      <c r="AW36" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="254"/>
+      <c r="AX36" s="256"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>
@@ -10208,10 +10476,10 @@
       <c r="BH36" s="65"/>
       <c r="BI36" s="65"/>
       <c r="BJ36" s="102"/>
-      <c r="BM36" s="253" t="s">
+      <c r="BM36" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="BN36" s="254"/>
+      <c r="BN36" s="256"/>
       <c r="BO36" s="9">
         <f>SUM(BM28:BN35)</f>
         <v>260</v>
@@ -10231,10 +10499,10 @@
     </row>
     <row r="37" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="255" t="s">
+      <c r="B38" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="257"/>
+      <c r="C38" s="259"/>
       <c r="D38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10274,10 +10542,10 @@
       <c r="P38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="S38" s="255" t="s">
+      <c r="S38" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="T38" s="257"/>
+      <c r="T38" s="259"/>
       <c r="U38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10317,11 +10585,11 @@
       <c r="AG38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="AJ38" s="255" t="s">
+      <c r="AJ38" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="AK38" s="256"/>
-      <c r="AL38" s="257"/>
+      <c r="AK38" s="258"/>
+      <c r="AL38" s="259"/>
       <c r="AM38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10364,13 +10632,13 @@
       <c r="AZ38" s="44"/>
       <c r="BA38" s="199">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
-      </c>
-      <c r="BD38" s="255" t="s">
+        <v>45292</v>
+      </c>
+      <c r="BD38" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="BE38" s="256"/>
-      <c r="BF38" s="257"/>
+      <c r="BE38" s="258"/>
+      <c r="BF38" s="259"/>
       <c r="BG38" s="26" t="s">
         <v>43</v>
       </c>
@@ -10410,11 +10678,11 @@
       <c r="BS38" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="BW38" s="255" t="s">
+      <c r="BW38" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="BX38" s="256"/>
-      <c r="BY38" s="257"/>
+      <c r="BX38" s="258"/>
+      <c r="BY38" s="259"/>
       <c r="BZ38" s="26" t="s">
         <v>43</v>
       </c>
@@ -11366,7 +11634,7 @@
     </row>
     <row r="44" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="163"/>
-      <c r="C44" s="290">
+      <c r="C44" s="283">
         <v>55</v>
       </c>
       <c r="D44" s="9" t="s">
@@ -11404,10 +11672,10 @@
       <c r="P44" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S44" s="283">
+      <c r="S44" s="292">
         <v>25</v>
       </c>
-      <c r="T44" s="290">
+      <c r="T44" s="283">
         <v>55</v>
       </c>
       <c r="U44" s="9" t="s">
@@ -11416,7 +11684,7 @@
       <c r="V44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="W44" s="285" t="s">
+      <c r="W44" s="286" t="s">
         <v>105</v>
       </c>
       <c r="X44" s="83" t="s">
@@ -11445,10 +11713,10 @@
       <c r="AG44" s="46" t="s">
         <v>160</v>
       </c>
-      <c r="AJ44" s="283">
+      <c r="AJ44" s="292">
         <v>50</v>
       </c>
-      <c r="AK44" s="290">
+      <c r="AK44" s="283">
         <v>10</v>
       </c>
       <c r="AL44" s="190"/>
@@ -11458,7 +11726,7 @@
       <c r="AN44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO44" s="285" t="s">
+      <c r="AO44" s="286" t="s">
         <v>105</v>
       </c>
       <c r="AP44" s="83" t="s">
@@ -11488,7 +11756,7 @@
         <v>168</v>
       </c>
       <c r="AZ44" s="49"/>
-      <c r="BD44" s="283">
+      <c r="BD44" s="292">
         <v>50</v>
       </c>
       <c r="BE44" s="208"/>
@@ -11499,7 +11767,7 @@
       <c r="BH44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI44" s="285" t="s">
+      <c r="BI44" s="286" t="s">
         <v>105</v>
       </c>
       <c r="BJ44" s="83" t="s">
@@ -11528,7 +11796,7 @@
       <c r="BS44" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW44" s="283">
+      <c r="BW44" s="292">
         <v>25</v>
       </c>
       <c r="BX44" s="208"/>
@@ -11539,7 +11807,7 @@
       <c r="CA44" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB44" s="285" t="s">
+      <c r="CB44" s="286" t="s">
         <v>105</v>
       </c>
       <c r="CC44" s="83" t="s">
@@ -11571,7 +11839,7 @@
     </row>
     <row r="45" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="140"/>
-      <c r="C45" s="291"/>
+      <c r="C45" s="284"/>
       <c r="D45" s="9" t="s">
         <v>71</v>
       </c>
@@ -11605,15 +11873,15 @@
       <c r="P45" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="S45" s="284"/>
-      <c r="T45" s="292"/>
+      <c r="S45" s="293"/>
+      <c r="T45" s="285"/>
       <c r="U45" s="9" t="s">
         <v>71</v>
       </c>
       <c r="V45" s="155" t="s">
         <v>17</v>
       </c>
-      <c r="W45" s="286"/>
+      <c r="W45" s="287"/>
       <c r="X45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11640,8 +11908,8 @@
       <c r="AG45" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="AJ45" s="284"/>
-      <c r="AK45" s="292"/>
+      <c r="AJ45" s="293"/>
+      <c r="AK45" s="285"/>
       <c r="AL45" s="191"/>
       <c r="AM45" s="9" t="s">
         <v>71</v>
@@ -11649,7 +11917,7 @@
       <c r="AN45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="AO45" s="286"/>
+      <c r="AO45" s="287"/>
       <c r="AP45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11677,7 +11945,7 @@
         <v>168</v>
       </c>
       <c r="AZ45" s="49"/>
-      <c r="BD45" s="284"/>
+      <c r="BD45" s="293"/>
       <c r="BE45" s="165">
         <v>20</v>
       </c>
@@ -11688,7 +11956,7 @@
       <c r="BH45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="BI45" s="286"/>
+      <c r="BI45" s="287"/>
       <c r="BJ45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11715,7 +11983,7 @@
       <c r="BS45" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="BW45" s="284"/>
+      <c r="BW45" s="293"/>
       <c r="BX45" s="165"/>
       <c r="BY45" s="191"/>
       <c r="BZ45" s="9" t="s">
@@ -11724,7 +11992,7 @@
       <c r="CA45" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="CB45" s="286"/>
+      <c r="CB45" s="287"/>
       <c r="CC45" s="182" t="s">
         <v>163</v>
       </c>
@@ -11754,7 +12022,7 @@
     </row>
     <row r="46" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="165"/>
-      <c r="C46" s="292"/>
+      <c r="C46" s="285"/>
       <c r="D46" s="9" t="s">
         <v>81</v>
       </c>
@@ -12181,10 +12449,10 @@
       </c>
     </row>
     <row r="48" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="253" t="s">
+      <c r="B48" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="254"/>
+      <c r="C48" s="256"/>
       <c r="D48" s="9">
         <f>SUM(B40:C47)</f>
         <v>200</v>
@@ -12203,10 +12471,10 @@
       <c r="N48" s="65"/>
       <c r="O48" s="65"/>
       <c r="P48" s="168"/>
-      <c r="S48" s="253" t="s">
+      <c r="S48" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="T48" s="254"/>
+      <c r="T48" s="256"/>
       <c r="U48" s="9">
         <f>SUM(S40:T47)</f>
         <v>296</v>
@@ -12359,11 +12627,11 @@
       <c r="AN49" s="25"/>
       <c r="AO49" s="119"/>
       <c r="AP49" s="119"/>
-      <c r="AQ49" s="287"/>
+      <c r="AQ49" s="288"/>
       <c r="AS49" s="192"/>
       <c r="AT49" s="2"/>
-      <c r="AU49" s="247"/>
-      <c r="AV49" s="248"/>
+      <c r="AU49" s="249"/>
+      <c r="AV49" s="250"/>
       <c r="AW49" s="1"/>
       <c r="AX49" s="1"/>
       <c r="AY49" s="24"/>
@@ -12375,11 +12643,11 @@
       <c r="BH49" s="25"/>
       <c r="BI49" s="119"/>
       <c r="BJ49" s="119"/>
-      <c r="BK49" s="287"/>
+      <c r="BK49" s="288"/>
       <c r="BM49" s="192"/>
       <c r="BN49" s="2"/>
-      <c r="BO49" s="247"/>
-      <c r="BP49" s="248"/>
+      <c r="BO49" s="249"/>
+      <c r="BP49" s="250"/>
       <c r="BQ49" s="1"/>
       <c r="BR49" s="1"/>
       <c r="BS49" s="46"/>
@@ -12390,20 +12658,20 @@
       <c r="CA49" s="25"/>
       <c r="CB49" s="119"/>
       <c r="CC49" s="119"/>
-      <c r="CD49" s="287"/>
+      <c r="CD49" s="288"/>
       <c r="CF49" s="192"/>
       <c r="CG49" s="2"/>
-      <c r="CH49" s="247"/>
-      <c r="CI49" s="248"/>
+      <c r="CH49" s="249"/>
+      <c r="CI49" s="250"/>
       <c r="CJ49" s="1"/>
       <c r="CK49" s="1"/>
       <c r="CL49" s="46"/>
     </row>
     <row r="50" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AJ50" s="253" t="s">
+      <c r="AJ50" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="AK50" s="254"/>
+      <c r="AK50" s="256"/>
       <c r="AL50" s="189" t="s">
         <v>179</v>
       </c>
@@ -12414,19 +12682,19 @@
       <c r="AN50" s="25"/>
       <c r="AO50" s="119"/>
       <c r="AP50" s="119"/>
-      <c r="AQ50" s="287"/>
+      <c r="AQ50" s="288"/>
       <c r="AS50" s="192"/>
       <c r="AT50" s="2"/>
-      <c r="AU50" s="247"/>
-      <c r="AV50" s="248"/>
+      <c r="AU50" s="249"/>
+      <c r="AV50" s="250"/>
       <c r="AW50" s="1"/>
       <c r="AX50" s="1"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="49"/>
-      <c r="BD50" s="253" t="s">
+      <c r="BD50" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="BE50" s="254"/>
+      <c r="BE50" s="256"/>
       <c r="BF50" s="189"/>
       <c r="BG50" s="9">
         <f>SUM(BD40:BF48)</f>
@@ -12435,18 +12703,18 @@
       <c r="BH50" s="25"/>
       <c r="BI50" s="119"/>
       <c r="BJ50" s="119"/>
-      <c r="BK50" s="287"/>
+      <c r="BK50" s="288"/>
       <c r="BM50" s="192"/>
       <c r="BN50" s="2"/>
-      <c r="BO50" s="247"/>
-      <c r="BP50" s="248"/>
+      <c r="BO50" s="249"/>
+      <c r="BP50" s="250"/>
       <c r="BQ50" s="1"/>
       <c r="BR50" s="1"/>
       <c r="BS50" s="46"/>
-      <c r="BW50" s="253" t="s">
+      <c r="BW50" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="BX50" s="254"/>
+      <c r="BX50" s="256"/>
       <c r="BY50" s="189"/>
       <c r="BZ50" s="9">
         <f>SUM(BW40:BY48)</f>
@@ -12455,21 +12723,21 @@
       <c r="CA50" s="25"/>
       <c r="CB50" s="119"/>
       <c r="CC50" s="119"/>
-      <c r="CD50" s="287"/>
+      <c r="CD50" s="288"/>
       <c r="CF50" s="192"/>
       <c r="CG50" s="2"/>
-      <c r="CH50" s="247"/>
-      <c r="CI50" s="248"/>
+      <c r="CH50" s="249"/>
+      <c r="CI50" s="250"/>
       <c r="CJ50" s="1"/>
       <c r="CK50" s="1"/>
       <c r="CL50" s="46"/>
     </row>
     <row r="51" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="255" t="s">
+      <c r="B51" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="256"/>
-      <c r="D51" s="257"/>
+      <c r="C51" s="258"/>
+      <c r="D51" s="259"/>
       <c r="E51" s="26" t="s">
         <v>43</v>
       </c>
@@ -12519,14 +12787,14 @@
       <c r="AN51" s="114"/>
       <c r="AO51" s="201"/>
       <c r="AP51" s="202"/>
-      <c r="AQ51" s="288"/>
+      <c r="AQ51" s="289"/>
       <c r="AR51" s="201"/>
       <c r="AS51" s="203"/>
       <c r="AT51" s="116" t="s">
         <v>160</v>
       </c>
-      <c r="AU51" s="289"/>
-      <c r="AV51" s="282"/>
+      <c r="AU51" s="290"/>
+      <c r="AV51" s="291"/>
       <c r="AW51" s="65"/>
       <c r="AX51" s="65"/>
       <c r="AY51" s="115"/>
@@ -12538,14 +12806,14 @@
       <c r="BH51" s="114"/>
       <c r="BI51" s="201"/>
       <c r="BJ51" s="202"/>
-      <c r="BK51" s="288"/>
+      <c r="BK51" s="289"/>
       <c r="BL51" s="201"/>
       <c r="BM51" s="203"/>
       <c r="BN51" s="79" t="s">
         <v>168</v>
       </c>
-      <c r="BO51" s="289"/>
-      <c r="BP51" s="282"/>
+      <c r="BO51" s="290"/>
+      <c r="BP51" s="291"/>
       <c r="BQ51" s="65"/>
       <c r="BR51" s="65"/>
       <c r="BS51" s="168"/>
@@ -12556,14 +12824,14 @@
       <c r="CA51" s="114"/>
       <c r="CB51" s="201"/>
       <c r="CC51" s="202"/>
-      <c r="CD51" s="288"/>
+      <c r="CD51" s="289"/>
       <c r="CE51" s="201"/>
       <c r="CF51" s="203" t="s">
         <v>180</v>
       </c>
       <c r="CG51" s="79"/>
-      <c r="CH51" s="289"/>
-      <c r="CI51" s="282"/>
+      <c r="CH51" s="290"/>
+      <c r="CI51" s="291"/>
       <c r="CJ51" s="65"/>
       <c r="CK51" s="65"/>
       <c r="CL51" s="168"/>
@@ -12584,11 +12852,11 @@
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="46"/>
-      <c r="V52" s="255" t="s">
+      <c r="V52" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="W52" s="256"/>
-      <c r="X52" s="257"/>
+      <c r="W52" s="258"/>
+      <c r="X52" s="259"/>
       <c r="Y52" s="26" t="s">
         <v>43</v>
       </c>
@@ -12690,11 +12958,11 @@
       <c r="AJ53" s="1"/>
       <c r="AK53" s="1"/>
       <c r="AL53" s="46"/>
-      <c r="AO53" s="255" t="s">
+      <c r="AO53" s="257" t="s">
         <v>145</v>
       </c>
-      <c r="AP53" s="256"/>
-      <c r="AQ53" s="257"/>
+      <c r="AP53" s="258"/>
+      <c r="AQ53" s="259"/>
       <c r="AR53" s="26" t="s">
         <v>43</v>
       </c>
@@ -12739,7 +13007,54 @@
       </c>
       <c r="BG53" s="98">
         <f ca="1">TODAY()</f>
-        <v>45291</v>
+        <v>45292</v>
+      </c>
+      <c r="BJ53" s="257" t="s">
+        <v>145</v>
+      </c>
+      <c r="BK53" s="258"/>
+      <c r="BL53" s="259"/>
+      <c r="BM53" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="BN53" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="BO53" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="BP53" s="214" t="s">
+        <v>195</v>
+      </c>
+      <c r="BQ53" s="83" t="s">
+        <v>153</v>
+      </c>
+      <c r="BR53" s="83" t="s">
+        <v>40</v>
+      </c>
+      <c r="BS53" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BT53" s="143" t="s">
+        <v>38</v>
+      </c>
+      <c r="BU53" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="BV53" s="153" t="s">
+        <v>68</v>
+      </c>
+      <c r="BW53" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="BX53" s="156" t="s">
+        <v>83</v>
+      </c>
+      <c r="BY53" s="214" t="s">
+        <v>224</v>
+      </c>
+      <c r="BZ53" s="36" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="54" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12843,6 +13158,23 @@
       <c r="BC54" s="1"/>
       <c r="BD54" s="1"/>
       <c r="BE54" s="46"/>
+      <c r="BJ54" s="136"/>
+      <c r="BK54" s="295"/>
+      <c r="BL54" s="296"/>
+      <c r="BM54" s="297"/>
+      <c r="BN54" s="298"/>
+      <c r="BO54" s="299"/>
+      <c r="BP54" s="300"/>
+      <c r="BQ54" s="299"/>
+      <c r="BR54" s="299"/>
+      <c r="BS54" s="297"/>
+      <c r="BT54" s="297"/>
+      <c r="BU54" s="296"/>
+      <c r="BV54" s="301"/>
+      <c r="BW54" s="295"/>
+      <c r="BX54" s="295"/>
+      <c r="BY54" s="295"/>
+      <c r="BZ54" s="46"/>
     </row>
     <row r="55" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="218"/>
@@ -12978,6 +13310,53 @@
       <c r="BE55" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ55" s="244">
+        <v>5</v>
+      </c>
+      <c r="BK55" s="205"/>
+      <c r="BL55" s="247">
+        <v>20</v>
+      </c>
+      <c r="BM55" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="BN55" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO55" s="213" t="s">
+        <v>187</v>
+      </c>
+      <c r="BP55" s="169" t="s">
+        <v>217</v>
+      </c>
+      <c r="BQ55" s="83" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR55" s="224" t="s">
+        <v>156</v>
+      </c>
+      <c r="BS55" s="143" t="s">
+        <v>193</v>
+      </c>
+      <c r="BT55" s="169" t="s">
+        <v>156</v>
+      </c>
+      <c r="BU55" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="BV55" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW55" s="295"/>
+      <c r="BX55" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY55" s="240">
+        <v>3</v>
+      </c>
+      <c r="BZ55" s="303">
+        <v>45292</v>
+      </c>
     </row>
     <row r="56" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="165"/>
@@ -13115,6 +13494,53 @@
       <c r="BE56" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ56" s="218">
+        <v>5</v>
+      </c>
+      <c r="BK56" s="206"/>
+      <c r="BL56" s="37">
+        <v>20</v>
+      </c>
+      <c r="BM56" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BN56" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO56" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="BP56" s="215" t="s">
+        <v>218</v>
+      </c>
+      <c r="BQ56" s="167" t="s">
+        <v>142</v>
+      </c>
+      <c r="BR56" s="224" t="s">
+        <v>85</v>
+      </c>
+      <c r="BS56" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="BT56" s="237" t="s">
+        <v>137</v>
+      </c>
+      <c r="BU56" s="197" t="s">
+        <v>86</v>
+      </c>
+      <c r="BV56" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW56" s="295"/>
+      <c r="BX56" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY56" s="238">
+        <v>1</v>
+      </c>
+      <c r="BZ56" s="303">
+        <v>45292</v>
+      </c>
     </row>
     <row r="57" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B57" s="219"/>
@@ -13248,6 +13674,53 @@
       <c r="BE57" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ57" s="218">
+        <v>5</v>
+      </c>
+      <c r="BK57" s="207"/>
+      <c r="BL57" s="127">
+        <v>40</v>
+      </c>
+      <c r="BM57" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="BN57" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO57" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="BP57" s="169" t="s">
+        <v>220</v>
+      </c>
+      <c r="BQ57" s="83" t="s">
+        <v>123</v>
+      </c>
+      <c r="BR57" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="BS57" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="BT57" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="BU57" s="176" t="s">
+        <v>69</v>
+      </c>
+      <c r="BV57" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW57" s="295"/>
+      <c r="BX57" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY57" s="240">
+        <v>3</v>
+      </c>
+      <c r="BZ57" s="303">
+        <v>45292</v>
+      </c>
     </row>
     <row r="58" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="163">
@@ -13380,6 +13853,55 @@
       </c>
       <c r="BE58" s="46" t="s">
         <v>223</v>
+      </c>
+      <c r="BJ58" s="165">
+        <v>10</v>
+      </c>
+      <c r="BK58" s="242"/>
+      <c r="BL58" s="177">
+        <v>10</v>
+      </c>
+      <c r="BM58" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="BN58" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO58" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="BP58" s="215" t="s">
+        <v>219</v>
+      </c>
+      <c r="BQ58" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="BR58" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="BS58" s="143" t="s">
+        <v>192</v>
+      </c>
+      <c r="BT58" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="BU58" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="BV58" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW58" s="295" t="s">
+        <v>130</v>
+      </c>
+      <c r="BX58" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY58" s="240">
+        <v>3</v>
+      </c>
+      <c r="BZ58" s="303">
+        <v>45292</v>
       </c>
     </row>
     <row r="59" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13506,6 +14028,49 @@
       <c r="BE59" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ59" s="219">
+        <v>75</v>
+      </c>
+      <c r="BK59" s="242"/>
+      <c r="BL59" s="190"/>
+      <c r="BM59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN59" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO59" s="213"/>
+      <c r="BP59" s="194" t="s">
+        <v>225</v>
+      </c>
+      <c r="BQ59" s="83" t="s">
+        <v>214</v>
+      </c>
+      <c r="BR59" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="BS59" s="187" t="s">
+        <v>196</v>
+      </c>
+      <c r="BT59" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU59" s="188" t="s">
+        <v>65</v>
+      </c>
+      <c r="BV59" s="302">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="BW59" s="295"/>
+      <c r="BX59" s="302">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="BY59" s="240">
+        <v>3</v>
+      </c>
+      <c r="BZ59" s="303">
+        <v>45292</v>
+      </c>
     </row>
     <row r="60" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="221">
@@ -13634,6 +14199,51 @@
       </c>
       <c r="BE60" s="46" t="s">
         <v>223</v>
+      </c>
+      <c r="BJ60" s="163">
+        <v>14</v>
+      </c>
+      <c r="BK60" s="165"/>
+      <c r="BL60" s="177"/>
+      <c r="BM60" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BN60" s="104" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO60" s="213" t="s">
+        <v>165</v>
+      </c>
+      <c r="BP60" s="169" t="s">
+        <v>215</v>
+      </c>
+      <c r="BQ60" s="223" t="s">
+        <v>163</v>
+      </c>
+      <c r="BR60" s="224" t="s">
+        <v>170</v>
+      </c>
+      <c r="BS60" s="143" t="s">
+        <v>191</v>
+      </c>
+      <c r="BT60" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="BU60" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="BV60" s="302">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="BW60" s="295"/>
+      <c r="BX60" s="302">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="BY60" s="239">
+        <v>1</v>
+      </c>
+      <c r="BZ60" s="303">
+        <v>45292</v>
       </c>
     </row>
     <row r="61" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13766,6 +14376,51 @@
       <c r="BE61" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ61" s="220">
+        <v>70</v>
+      </c>
+      <c r="BK61" s="206"/>
+      <c r="BL61" s="177">
+        <v>7</v>
+      </c>
+      <c r="BM61" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="BN61" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO61" s="213"/>
+      <c r="BP61" s="169" t="s">
+        <v>222</v>
+      </c>
+      <c r="BQ61" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="BR61" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS61" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="BT61" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="BU61" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="BV61" s="302">
+        <v>0.625</v>
+      </c>
+      <c r="BW61" s="295"/>
+      <c r="BX61" s="302">
+        <v>0.625</v>
+      </c>
+      <c r="BY61" s="240">
+        <v>6</v>
+      </c>
+      <c r="BZ61" s="303">
+        <v>45292</v>
+      </c>
     </row>
     <row r="62" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="36">
@@ -13901,6 +14556,57 @@
       </c>
       <c r="BE62" s="46" t="s">
         <v>223</v>
+      </c>
+      <c r="BJ62" s="221">
+        <v>5</v>
+      </c>
+      <c r="BK62" s="242">
+        <v>20</v>
+      </c>
+      <c r="BL62" s="37">
+        <v>10</v>
+      </c>
+      <c r="BM62" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="BN62" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO62" s="213" t="s">
+        <v>116</v>
+      </c>
+      <c r="BP62" s="194" t="s">
+        <v>226</v>
+      </c>
+      <c r="BQ62" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="BR62" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="BS62" s="186" t="s">
+        <v>110</v>
+      </c>
+      <c r="BT62" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="BU62" s="198" t="s">
+        <v>161</v>
+      </c>
+      <c r="BV62" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW62" s="295" t="s">
+        <v>126</v>
+      </c>
+      <c r="BX62" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY62" s="241">
+        <v>1</v>
+      </c>
+      <c r="BZ62" s="303">
+        <v>45292</v>
       </c>
     </row>
     <row r="63" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14026,6 +14732,51 @@
       </c>
       <c r="BE63" s="46" t="s">
         <v>223</v>
+      </c>
+      <c r="BJ63" s="165">
+        <v>10</v>
+      </c>
+      <c r="BK63" s="205"/>
+      <c r="BL63" s="164">
+        <v>200</v>
+      </c>
+      <c r="BM63" s="304" t="s">
+        <v>128</v>
+      </c>
+      <c r="BN63" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO63" s="213"/>
+      <c r="BP63" s="169" t="s">
+        <v>221</v>
+      </c>
+      <c r="BQ63" s="224" t="s">
+        <v>123</v>
+      </c>
+      <c r="BR63" s="225" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS63" s="143" t="s">
+        <v>197</v>
+      </c>
+      <c r="BT63" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="BU63" s="188" t="s">
+        <v>181</v>
+      </c>
+      <c r="BV63" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW63" s="305"/>
+      <c r="BX63" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY63" s="238">
+        <v>3</v>
+      </c>
+      <c r="BZ63" s="303">
+        <v>45292</v>
       </c>
     </row>
     <row r="64" spans="2:90" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14146,8 +14897,55 @@
       <c r="BE64" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ64" s="36">
+        <v>1</v>
+      </c>
+      <c r="BK64" s="206"/>
+      <c r="BL64" s="246">
+        <v>25</v>
+      </c>
+      <c r="BM64" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="BN64" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO64" s="228" t="s">
+        <v>186</v>
+      </c>
+      <c r="BP64" s="194" t="s">
+        <v>208</v>
+      </c>
+      <c r="BQ64" s="183" t="s">
+        <v>155</v>
+      </c>
+      <c r="BR64" s="183" t="s">
+        <v>85</v>
+      </c>
+      <c r="BS64" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT64" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="BU64" s="229" t="s">
+        <v>90</v>
+      </c>
+      <c r="BV64" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BW64" s="297"/>
+      <c r="BX64" s="302">
+        <v>0.88611111111111107</v>
+      </c>
+      <c r="BY64" s="243">
+        <v>1</v>
+      </c>
+      <c r="BZ64" s="303">
+        <v>45292</v>
+      </c>
     </row>
-    <row r="65" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="136"/>
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
@@ -14230,12 +15028,49 @@
       <c r="BE65" s="46" t="s">
         <v>223</v>
       </c>
+      <c r="BJ65" s="165">
+        <v>10</v>
+      </c>
+      <c r="BK65" s="205"/>
+      <c r="BL65" s="184"/>
+      <c r="BM65" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BN65" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO65" s="213"/>
+      <c r="BP65" s="169" t="s">
+        <v>227</v>
+      </c>
+      <c r="BQ65" s="83" t="s">
+        <v>124</v>
+      </c>
+      <c r="BR65" s="224"/>
+      <c r="BS65" s="143" t="s">
+        <v>200</v>
+      </c>
+      <c r="BT65" s="169"/>
+      <c r="BU65" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="BV65" s="302">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="BW65" s="297"/>
+      <c r="BX65" s="302">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="BY65" s="295"/>
+      <c r="BZ65" s="303">
+        <v>45292</v>
+      </c>
     </row>
-    <row r="66" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="253" t="s">
+    <row r="66" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="C66" s="254"/>
+      <c r="C66" s="256"/>
       <c r="D66" s="189"/>
       <c r="E66" s="9">
         <f>SUM(B53:D64)</f>
@@ -14248,8 +15083,8 @@
       <c r="J66" s="117"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
-      <c r="N66" s="247"/>
-      <c r="O66" s="248"/>
+      <c r="N66" s="249"/>
+      <c r="O66" s="250"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="46"/>
@@ -14295,8 +15130,37 @@
       <c r="BE66" s="46" t="s">
         <v>184</v>
       </c>
+      <c r="BJ66" s="165"/>
+      <c r="BK66" s="34"/>
+      <c r="BL66" s="177"/>
+      <c r="BM66" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="BN66" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BO66" s="231"/>
+      <c r="BP66" s="169"/>
+      <c r="BQ66" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="BR66" s="233"/>
+      <c r="BS66" s="9"/>
+      <c r="BT66" s="8"/>
+      <c r="BU66" s="37"/>
+      <c r="BV66" s="302">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="BW66" s="297"/>
+      <c r="BX66" s="302">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="BY66" s="305"/>
+      <c r="BZ66" s="303">
+        <v>45292</v>
+      </c>
     </row>
-    <row r="67" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="235"/>
       <c r="C67" s="24"/>
       <c r="D67" s="20"/>
@@ -14304,18 +15168,18 @@
       <c r="G67" s="119"/>
       <c r="H67" s="216"/>
       <c r="I67" s="119"/>
-      <c r="J67" s="246"/>
+      <c r="J67" s="248"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
-      <c r="N67" s="247"/>
-      <c r="O67" s="248"/>
+      <c r="N67" s="249"/>
+      <c r="O67" s="250"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
       <c r="R67" s="46"/>
-      <c r="V67" s="253" t="s">
+      <c r="V67" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="W67" s="254"/>
+      <c r="W67" s="256"/>
       <c r="X67" s="189"/>
       <c r="Y67" s="9">
         <f>SUM(V54:X65)</f>
@@ -14327,8 +15191,8 @@
       <c r="AC67" s="119"/>
       <c r="AD67" s="117"/>
       <c r="AG67" s="2"/>
-      <c r="AH67" s="247"/>
-      <c r="AI67" s="248"/>
+      <c r="AH67" s="249"/>
+      <c r="AI67" s="250"/>
       <c r="AJ67" s="1"/>
       <c r="AK67" s="1"/>
       <c r="AL67" s="46"/>
@@ -14346,8 +15210,25 @@
       <c r="BC67" s="1"/>
       <c r="BD67" s="1"/>
       <c r="BE67" s="46"/>
+      <c r="BJ67" s="136"/>
+      <c r="BK67" s="295"/>
+      <c r="BL67" s="296"/>
+      <c r="BM67" s="297"/>
+      <c r="BN67" s="234"/>
+      <c r="BO67" s="306"/>
+      <c r="BP67" s="307"/>
+      <c r="BQ67" s="306"/>
+      <c r="BR67" s="299"/>
+      <c r="BS67" s="297"/>
+      <c r="BT67" s="297"/>
+      <c r="BU67" s="296"/>
+      <c r="BV67" s="301"/>
+      <c r="BW67" s="295"/>
+      <c r="BX67" s="295"/>
+      <c r="BY67" s="295"/>
+      <c r="BZ67" s="46"/>
     </row>
-    <row r="68" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="236"/>
       <c r="C68" s="65"/>
       <c r="D68" s="79"/>
@@ -14356,7 +15237,7 @@
       <c r="G68" s="137"/>
       <c r="H68" s="203"/>
       <c r="I68" s="137"/>
-      <c r="J68" s="281"/>
+      <c r="J68" s="294"/>
       <c r="K68" s="50"/>
       <c r="L68" s="79"/>
       <c r="M68" s="79"/>
@@ -14372,17 +15253,17 @@
       <c r="AA68" s="119"/>
       <c r="AB68" s="216"/>
       <c r="AC68" s="119"/>
-      <c r="AD68" s="246"/>
+      <c r="AD68" s="248"/>
       <c r="AG68" s="2"/>
-      <c r="AH68" s="247"/>
-      <c r="AI68" s="248"/>
+      <c r="AH68" s="249"/>
+      <c r="AI68" s="250"/>
       <c r="AJ68" s="1"/>
       <c r="AK68" s="1"/>
       <c r="AL68" s="46"/>
-      <c r="AO68" s="253" t="s">
+      <c r="AO68" s="255" t="s">
         <v>4</v>
       </c>
-      <c r="AP68" s="254"/>
+      <c r="AP68" s="256"/>
       <c r="AQ68" s="189"/>
       <c r="AR68" s="9">
         <f>SUM(AO55:AQ66)</f>
@@ -14394,13 +15275,35 @@
       <c r="AV68" s="119"/>
       <c r="AW68" s="117"/>
       <c r="AZ68" s="2"/>
-      <c r="BA68" s="247"/>
-      <c r="BB68" s="248"/>
+      <c r="BA68" s="249"/>
+      <c r="BB68" s="250"/>
       <c r="BC68" s="1"/>
       <c r="BD68" s="1"/>
       <c r="BE68" s="46"/>
+      <c r="BJ68" s="255" t="s">
+        <v>4</v>
+      </c>
+      <c r="BK68" s="256"/>
+      <c r="BL68" s="189"/>
+      <c r="BM68" s="9">
+        <f>SUM(BJ55:BL66)</f>
+        <v>562</v>
+      </c>
+      <c r="BN68" s="26"/>
+      <c r="BO68" s="306"/>
+      <c r="BP68" s="307"/>
+      <c r="BQ68" s="306"/>
+      <c r="BR68" s="299"/>
+      <c r="BS68" s="297"/>
+      <c r="BT68" s="297"/>
+      <c r="BU68" s="296"/>
+      <c r="BV68" s="308"/>
+      <c r="BW68" s="309"/>
+      <c r="BX68" s="295"/>
+      <c r="BY68" s="295"/>
+      <c r="BZ68" s="46"/>
     </row>
-    <row r="69" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="V69" s="236"/>
       <c r="W69" s="65"/>
       <c r="X69" s="79"/>
@@ -14411,7 +15314,7 @@
       <c r="AC69" s="137" t="s">
         <v>184</v>
       </c>
-      <c r="AD69" s="281"/>
+      <c r="AD69" s="294"/>
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
       <c r="AG69" s="79"/>
@@ -14427,15 +15330,32 @@
       <c r="AT69" s="119"/>
       <c r="AU69" s="192"/>
       <c r="AV69" s="119"/>
-      <c r="AW69" s="246"/>
+      <c r="AW69" s="248"/>
       <c r="AZ69" s="2"/>
-      <c r="BA69" s="247"/>
-      <c r="BB69" s="248"/>
+      <c r="BA69" s="249"/>
+      <c r="BB69" s="250"/>
       <c r="BC69" s="1"/>
       <c r="BD69" s="1"/>
       <c r="BE69" s="46"/>
+      <c r="BJ69" s="235"/>
+      <c r="BK69" s="305"/>
+      <c r="BL69" s="310"/>
+      <c r="BM69" s="297"/>
+      <c r="BN69" s="226"/>
+      <c r="BO69" s="306"/>
+      <c r="BP69" s="300"/>
+      <c r="BQ69" s="306"/>
+      <c r="BR69" s="311"/>
+      <c r="BS69" s="297"/>
+      <c r="BT69" s="297"/>
+      <c r="BU69" s="296"/>
+      <c r="BV69" s="308"/>
+      <c r="BW69" s="309"/>
+      <c r="BX69" s="295"/>
+      <c r="BY69" s="295"/>
+      <c r="BZ69" s="46"/>
     </row>
-    <row r="70" spans="2:57" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:78" x14ac:dyDescent="0.25">
       <c r="AO70" s="136"/>
       <c r="AP70" s="1"/>
       <c r="AQ70" s="2"/>
@@ -14443,15 +15363,32 @@
       <c r="AT70" s="117"/>
       <c r="AU70" s="192"/>
       <c r="AV70" s="119"/>
-      <c r="AW70" s="246"/>
+      <c r="AW70" s="248"/>
       <c r="AZ70" s="2"/>
       <c r="BA70" s="152"/>
       <c r="BB70" s="1"/>
       <c r="BC70" s="1"/>
       <c r="BD70" s="1"/>
       <c r="BE70" s="46"/>
+      <c r="BJ70" s="136"/>
+      <c r="BK70" s="295"/>
+      <c r="BL70" s="296"/>
+      <c r="BM70" s="297"/>
+      <c r="BN70" s="226"/>
+      <c r="BO70" s="299"/>
+      <c r="BP70" s="300"/>
+      <c r="BQ70" s="306"/>
+      <c r="BR70" s="311"/>
+      <c r="BS70" s="297"/>
+      <c r="BT70" s="297"/>
+      <c r="BU70" s="296"/>
+      <c r="BV70" s="301"/>
+      <c r="BW70" s="295"/>
+      <c r="BX70" s="295"/>
+      <c r="BY70" s="295"/>
+      <c r="BZ70" s="46"/>
     </row>
-    <row r="71" spans="2:57" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AO71" s="236"/>
       <c r="AP71" s="65"/>
       <c r="AQ71" s="79"/>
@@ -14471,25 +15408,60 @@
       <c r="BC71" s="65"/>
       <c r="BD71" s="65"/>
       <c r="BE71" s="168"/>
+      <c r="BJ71" s="236"/>
+      <c r="BK71" s="65"/>
+      <c r="BL71" s="79"/>
+      <c r="BM71" s="50"/>
+      <c r="BN71" s="227"/>
+      <c r="BO71" s="137"/>
+      <c r="BP71" s="203"/>
+      <c r="BQ71" s="201"/>
+      <c r="BR71" s="137"/>
+      <c r="BS71" s="50"/>
+      <c r="BT71" s="50"/>
+      <c r="BU71" s="79"/>
+      <c r="BV71" s="230"/>
+      <c r="BW71" s="65"/>
+      <c r="BX71" s="65"/>
+      <c r="BY71" s="65"/>
+      <c r="BZ71" s="168"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="S48:T48"/>
-    <mergeCell ref="AO44:AO45"/>
-    <mergeCell ref="AQ49:AQ51"/>
-    <mergeCell ref="AU49:AU51"/>
-    <mergeCell ref="AV49:AV51"/>
-    <mergeCell ref="AJ50:AK50"/>
-    <mergeCell ref="S38:T38"/>
-    <mergeCell ref="S44:S45"/>
-    <mergeCell ref="T44:T45"/>
-    <mergeCell ref="W44:W45"/>
-    <mergeCell ref="AJ38:AL38"/>
-    <mergeCell ref="AJ44:AJ45"/>
-    <mergeCell ref="AK44:AK45"/>
+  <mergeCells count="65">
+    <mergeCell ref="BJ53:BL53"/>
+    <mergeCell ref="BJ68:BK68"/>
+    <mergeCell ref="BV68:BV69"/>
+    <mergeCell ref="BW68:BW69"/>
+    <mergeCell ref="BR69:BR70"/>
+    <mergeCell ref="AO53:AQ53"/>
+    <mergeCell ref="AO68:AP68"/>
+    <mergeCell ref="BA68:BA69"/>
+    <mergeCell ref="BB68:BB69"/>
+    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="V52:X52"/>
+    <mergeCell ref="V67:W67"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AI67:AI68"/>
+    <mergeCell ref="AD68:AD69"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="N66:N67"/>
+    <mergeCell ref="O66:O67"/>
+    <mergeCell ref="J67:J68"/>
+    <mergeCell ref="CI49:CI51"/>
+    <mergeCell ref="BW50:BX50"/>
+    <mergeCell ref="BW38:BY38"/>
+    <mergeCell ref="BW44:BW45"/>
+    <mergeCell ref="CB44:CB45"/>
+    <mergeCell ref="CD49:CD51"/>
+    <mergeCell ref="CH49:CH51"/>
+    <mergeCell ref="BP49:BP51"/>
+    <mergeCell ref="BD50:BE50"/>
+    <mergeCell ref="BD38:BF38"/>
+    <mergeCell ref="BD44:BD45"/>
+    <mergeCell ref="BI44:BI45"/>
+    <mergeCell ref="BK49:BK51"/>
+    <mergeCell ref="BO49:BO51"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
@@ -14505,35 +15477,22 @@
     <mergeCell ref="BM36:BN36"/>
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
-    <mergeCell ref="BP49:BP51"/>
-    <mergeCell ref="BD50:BE50"/>
-    <mergeCell ref="BD38:BF38"/>
-    <mergeCell ref="BD44:BD45"/>
-    <mergeCell ref="BI44:BI45"/>
-    <mergeCell ref="BK49:BK51"/>
-    <mergeCell ref="BO49:BO51"/>
-    <mergeCell ref="CI49:CI51"/>
-    <mergeCell ref="BW50:BX50"/>
-    <mergeCell ref="BW38:BY38"/>
-    <mergeCell ref="BW44:BW45"/>
-    <mergeCell ref="CB44:CB45"/>
-    <mergeCell ref="CD49:CD51"/>
-    <mergeCell ref="CH49:CH51"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="N66:N67"/>
-    <mergeCell ref="O66:O67"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="V52:X52"/>
-    <mergeCell ref="V67:W67"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AI67:AI68"/>
-    <mergeCell ref="AD68:AD69"/>
-    <mergeCell ref="AO53:AQ53"/>
-    <mergeCell ref="AO68:AP68"/>
-    <mergeCell ref="BA68:BA69"/>
-    <mergeCell ref="BB68:BB69"/>
-    <mergeCell ref="AW69:AW70"/>
+    <mergeCell ref="AQ49:AQ51"/>
+    <mergeCell ref="AU49:AU51"/>
+    <mergeCell ref="AV49:AV51"/>
+    <mergeCell ref="AJ50:AK50"/>
+    <mergeCell ref="S38:T38"/>
+    <mergeCell ref="S44:S45"/>
+    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="W44:W45"/>
+    <mergeCell ref="AJ38:AL38"/>
+    <mergeCell ref="AJ44:AJ45"/>
+    <mergeCell ref="AK44:AK45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="S48:T48"/>
+    <mergeCell ref="AO44:AO45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>